<commit_message>
table 3 done, need to check
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="70">
   <si>
     <t>Secchi depth (m)</t>
   </si>
@@ -343,11 +344,123 @@
       <t xml:space="preserve"> (Peres-Neto et al. 2006) from partial redundancy analysis, partial least squares, and generalized linear models.  </t>
     </r>
   </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>prec</t>
+  </si>
+  <si>
+    <t>tmax</t>
+  </si>
+  <si>
+    <t>tmean</t>
+  </si>
+  <si>
+    <t>tmin</t>
+  </si>
+  <si>
+    <t>alk</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>secchi</t>
+  </si>
+  <si>
+    <t>tp</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>***+</t>
+  </si>
+  <si>
+    <t>***-</t>
+  </si>
+  <si>
+    <t>*+</t>
+  </si>
+  <si>
+    <t>**-</t>
+  </si>
+  <si>
+    <t>ns-</t>
+  </si>
+  <si>
+    <t>*-</t>
+  </si>
+  <si>
+    <t>ns+</t>
+  </si>
+  <si>
+    <t>**+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>Table 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Significant explanatory variables (i.e. local, climate and space variables) demonstrated by forward and backward selection based on AIC. Direction of the effect is indicated by + and − symbols.  Empty space means that the variable was not selected for the response. For spatial variables, only the number of selected significant eigenvectors is shown. Explaied deviance (%) indicates how much the model explains the dependent variable based on adjusted R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>. ***: p ≤ 0.0001, **: p ≤ 0.001, *: p≤ 0.05, ns: p &gt; 0.05.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -443,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -465,15 +578,6 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,6 +591,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,13 +910,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1043,56 +1171,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.28515625" style="14" customWidth="1"/>
-    <col min="5" max="7" width="15.85546875" style="14" customWidth="1"/>
-    <col min="8" max="9" width="12.28515625" style="14" customWidth="1"/>
+    <col min="2" max="4" width="8.28515625" style="11" customWidth="1"/>
+    <col min="5" max="7" width="15.85546875" style="11" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" style="11" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1100,28 +1228,28 @@
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="12">
         <v>5.6386745782657197</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>1.6275357165656901</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <v>2.0967423638908498</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="12">
         <v>2.4015463441952001</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="12">
         <v>3.2803663428180099</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="12">
         <v>1.02568751302806</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="12">
         <v>8.5840061655936903</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="12">
         <v>75.345440975642802</v>
       </c>
     </row>
@@ -1129,28 +1257,28 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>3.3396268152061399</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>1.06522898396133</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>2.2913515460082099</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="12">
         <v>6.7293483232064002</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="12">
         <v>-0.210375231957283</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="12">
         <v>2.7673894114881299</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="12">
         <v>-3.2879506166974699</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="12">
         <v>87.305380768784502</v>
       </c>
     </row>
@@ -1158,28 +1286,28 @@
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>5.4330505108965603</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>-0.28100686998880903</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>0.165494611875838</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <v>-0.40948826046377501</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="12">
         <v>-0.36637928818973298</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="12">
         <v>1.70622821583962</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="12">
         <v>9.1079511312440395</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="12">
         <v>84.644149948786307</v>
       </c>
     </row>
@@ -1187,28 +1315,28 @@
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>1.0392002254961701</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>0.84480128988587699</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>16.465481084219</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>-0.144698976403179</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="12">
         <v>7.75631428758801</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="12">
         <v>0.50366521496688599</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="12">
         <v>2.2250029703380001</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="12">
         <v>71.310233903909193</v>
       </c>
     </row>
@@ -1216,28 +1344,28 @@
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>6.2824138637025504</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>0.74541518006422403</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>-4.6160969394618698</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>0.48586050517387402</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <v>2.6073084105503499</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="12">
         <v>4.9132645695611199</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="12">
         <v>6.0019959337168496</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="12">
         <v>83.579838476692899</v>
       </c>
     </row>
@@ -1245,28 +1373,28 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>17.910148526701398</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>1.1083968276877101</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>-1.79287926682863</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>0.81450770493332003</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <v>2.1348587332625999</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="12">
         <v>0.38139458528203601</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="12">
         <v>5.7198704785400301</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="12">
         <v>73.723702410421495</v>
       </c>
     </row>
@@ -1274,28 +1402,28 @@
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>8.8134219891704202</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>-0.64816652801144004</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>13.5650399394255</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>0.49678318884715</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="12">
         <v>1.5309802917134601</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="12">
         <v>1.5205013533887799</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="12">
         <v>3.3323085194736302</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="12">
         <v>71.389131245992502</v>
       </c>
     </row>
@@ -1303,28 +1431,28 @@
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>11.038929370899099</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>-0.85952890366055601</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>11.6399202863439</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>-0.28622742826535102</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="12">
         <v>8.6206279641520904</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="12">
         <v>0.94569056321130995</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="12">
         <v>8.8032911080238492</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="12">
         <v>60.097297039295697</v>
       </c>
     </row>
@@ -1332,28 +1460,28 @@
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <v>2.9560568124720499</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>-0.30230983747199203</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>2.8574640970501601</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>0.61435127672913004</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="12">
         <v>8.0357152152810099E-2</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <v>-0.13460052071433401</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="12">
         <v>-7.8410889832669597E-2</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="12">
         <v>94.0070919096148</v>
       </c>
     </row>
@@ -1361,28 +1489,28 @@
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>-1.22459924325595</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>-2.7831533511508502</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>-9.6946532652051491</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>0.45751856260178903</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="12">
         <v>2.49005024751736</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="12">
         <v>4.7001081856666298</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="12">
         <v>1.0173591827091</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="12">
         <v>105.037369681117</v>
       </c>
     </row>
@@ -1390,28 +1518,28 @@
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <v>4.73821131688333</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>3.08013990558229</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>5.5685627267099402</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <v>-4.1877386942900801</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="12">
         <v>0.91586705484203401</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="12">
         <v>1.18335620101512</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="12">
         <v>-1.0001723039772601</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="12">
         <v>89.701773793234594</v>
       </c>
     </row>
@@ -1419,28 +1547,28 @@
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>6.6672555496199504</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>0.804356685193652</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>3.9971516577555501</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>-0.16136630994804099</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <v>-6.9495546791320501E-2</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="12">
         <v>5.2245215960010896</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="12">
         <v>3.5804331170533801</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="12">
         <v>79.957143251115696</v>
       </c>
     </row>
@@ -1448,28 +1576,28 @@
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="12">
         <v>11.561107195252699</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>2.2932814506523602</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>-6.1303440583693199E-2</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="12">
         <v>-0.18070355244274</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="12">
         <v>10.519443105119599</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="12">
         <v>-4.8916245028243104</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="12">
         <v>9.2658562907152504</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="12">
         <v>71.493943454110905</v>
       </c>
     </row>
@@ -1477,28 +1605,28 @@
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="12">
         <v>11.4343596042175</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>0.37079626074427702</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <v>3.0619872219749</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="12">
         <v>0.26278237492135498</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="12">
         <v>-1.52498309817262</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="12">
         <v>0.32221144128914397</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="12">
         <v>2.0129848248386</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="12">
         <v>84.059861370186795</v>
       </c>
     </row>
@@ -1506,28 +1634,28 @@
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="12">
         <v>2.2489799557933199</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>2.0463138448605802</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>12.3640502452019</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="12">
         <v>0.36781546095963102</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="12">
         <v>1.5227937950844199</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="12">
         <v>3.7369799778971502</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="12">
         <v>14.154852752778901</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="12">
         <v>63.558213967424102</v>
       </c>
     </row>
@@ -1535,28 +1663,28 @@
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="12">
         <v>3.9548674716817098</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="12">
         <v>3.3094215991238101</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="12">
         <v>4.5888724929466296</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="12">
         <v>5.1231559814727801</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="12">
         <v>-2.3268816893273199</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="12">
         <v>4.3812945467850097</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="12">
         <v>0.304605872598118</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="12">
         <v>80.664663724719304</v>
       </c>
     </row>
@@ -1564,57 +1692,57 @@
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="12">
         <v>1.55018273989375</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="12">
         <v>1.9417504342040599</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="12">
         <v>-1.95461849362608</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="12">
         <v>0.232766226269432</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="12">
         <v>0.88341686931632202</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="12">
         <v>0.51909796918715401</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="12">
         <v>2.23186388402498</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="12">
         <v>94.595540370730404</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="14">
         <v>10.524136364312</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="14">
         <v>-1.2615784287398499</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="14">
         <v>10.4193855544587</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="14">
         <v>-0.20139114680287601</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="14">
         <v>3.2559715885348801</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="14">
         <v>0.55165030886301603</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="14">
         <v>6.0854995011881003</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="14">
         <v>70.626326258185998</v>
       </c>
     </row>
@@ -1825,4 +1953,947 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22">
+        <v>13.813000994394899</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="21"/>
+      <c r="N4" s="22">
+        <v>7.3930744382742297</v>
+      </c>
+      <c r="O4" s="21">
+        <v>7</v>
+      </c>
+      <c r="P4" s="22">
+        <v>15.010234071807099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="22">
+        <v>4.7314987271284403</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="22">
+        <v>6.9260625091699701</v>
+      </c>
+      <c r="O5" s="21">
+        <v>47</v>
+      </c>
+      <c r="P5" s="22">
+        <v>25.7500832051049</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="22">
+        <v>14.5459147224738</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22">
+        <v>1.5476890131158301</v>
+      </c>
+      <c r="O6" s="21">
+        <v>48</v>
+      </c>
+      <c r="P6" s="22">
+        <v>32.472596635985802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="22">
+        <v>21.9680592555085</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="22">
+        <v>43.397815716435701</v>
+      </c>
+      <c r="O7" s="21">
+        <v>44</v>
+      </c>
+      <c r="P7" s="22">
+        <v>66.628412305160296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22">
+        <v>46.869703576928003</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" s="21"/>
+      <c r="N8" s="22">
+        <v>18.723486491219699</v>
+      </c>
+      <c r="O8" s="21">
+        <v>29</v>
+      </c>
+      <c r="P8" s="22">
+        <v>65.118829886833495</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22">
+        <v>50.902543885127599</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="22">
+        <v>30.5730171973042</v>
+      </c>
+      <c r="O9" s="21">
+        <v>2</v>
+      </c>
+      <c r="P9" s="22">
+        <v>99.999998289872494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="22">
+        <v>7.2318882400686002</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="N10" s="22">
+        <v>10.761138053583</v>
+      </c>
+      <c r="O10" s="21">
+        <v>47</v>
+      </c>
+      <c r="P10" s="22">
+        <v>44.277304399635398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="22">
+        <v>13.0453089858563</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="N11" s="22">
+        <v>13.180275148516399</v>
+      </c>
+      <c r="O11" s="21">
+        <v>41</v>
+      </c>
+      <c r="P11" s="22">
+        <v>32.027133493186298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="22">
+        <v>30.3027051145265</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22">
+        <v>16.820689566885299</v>
+      </c>
+      <c r="O12" s="21">
+        <v>48</v>
+      </c>
+      <c r="P12" s="22">
+        <v>61.150251021438599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="22">
+        <v>20.543576653187301</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="N13" s="22">
+        <v>37.865641231842197</v>
+      </c>
+      <c r="O13" s="21">
+        <v>40</v>
+      </c>
+      <c r="P13" s="22">
+        <v>61.353189192038201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22">
+        <v>99.999994948098703</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14" s="22">
+        <v>26.648493516007399</v>
+      </c>
+      <c r="O14" s="21">
+        <v>2</v>
+      </c>
+      <c r="P14" s="22">
+        <v>97.5799616212676</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22">
+        <v>45.626916354184097</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" s="22">
+        <v>44.023978604520202</v>
+      </c>
+      <c r="O15" s="21">
+        <v>44</v>
+      </c>
+      <c r="P15" s="22">
+        <v>70.204150781730704</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="22">
+        <v>6.3640842062335601</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" s="22">
+        <v>11.2665347659867</v>
+      </c>
+      <c r="O16" s="21">
+        <v>49</v>
+      </c>
+      <c r="P16" s="22">
+        <v>46.626418187891701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="22">
+        <v>43.426424649990203</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="22">
+        <v>41.570253763039901</v>
+      </c>
+      <c r="O17" s="21">
+        <v>37</v>
+      </c>
+      <c r="P17" s="22">
+        <v>61.114729642958899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="22">
+        <v>1.8111201528302701</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" s="22">
+        <v>3.1391554467821199</v>
+      </c>
+      <c r="O18" s="21">
+        <v>45</v>
+      </c>
+      <c r="P18" s="22">
+        <v>24.250328135362601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="22">
+        <v>26.485517092593099</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" s="22">
+        <v>4.2849073811194698</v>
+      </c>
+      <c r="O19" s="21">
+        <v>52</v>
+      </c>
+      <c r="P19" s="22">
+        <v>57.000252610546603</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="22">
+        <v>34.844867065611297</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" s="22">
+        <v>20.0522858049662</v>
+      </c>
+      <c r="O20" s="21">
+        <v>32</v>
+      </c>
+      <c r="P20" s="22">
+        <v>67.831021136782496</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="24">
+        <v>5.9332010456594997</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="24">
+        <v>14.5205420240063</v>
+      </c>
+      <c r="O21" s="23">
+        <v>44</v>
+      </c>
+      <c r="P21" s="24">
+        <v>32.641022257387398</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="A1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tables updated, figs 1 through six done
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -12,9 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
   <si>
     <t>Secchi depth (m)</t>
   </si>
@@ -279,9 +279,6 @@
   </si>
   <si>
     <t>Space</t>
-  </si>
-  <si>
-    <t>Unexplained</t>
   </si>
   <si>
     <t>P. filiformis</t>
@@ -452,6 +449,18 @@
       </rPr>
       <t>. ***: p ≤ 0.0001, **: p ≤ 0.001, *: p≤ 0.05, ns: p &gt; 0.05.</t>
     </r>
+  </si>
+  <si>
+    <t>P. foliosus</t>
+  </si>
+  <si>
+    <t>P. nodosus</t>
+  </si>
+  <si>
+    <t>P. spirillus</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -592,6 +601,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -602,18 +623,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -910,13 +919,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1169,7 +1178,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -1185,17 +1194,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="A1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
@@ -1221,7 +1230,7 @@
         <v>34</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1229,28 +1238,28 @@
         <v>20</v>
       </c>
       <c r="B3" s="12">
-        <v>5.6386745782657197</v>
+        <v>5.1456982490132397</v>
       </c>
       <c r="C3" s="12">
-        <v>1.6275357165656901</v>
+        <v>1.5869537129996201</v>
       </c>
       <c r="D3" s="12">
-        <v>2.0967423638908498</v>
+        <v>3.11118148815908</v>
       </c>
       <c r="E3" s="12">
-        <v>2.4015463441952001</v>
+        <v>1.92620089385493</v>
       </c>
       <c r="F3" s="12">
-        <v>3.2803663428180099</v>
+        <v>3.3209483463840801</v>
       </c>
       <c r="G3" s="12">
-        <v>1.02568751302806</v>
+        <v>1.5186638422805401</v>
       </c>
       <c r="H3" s="12">
-        <v>8.5840061655936903</v>
+        <v>9.0593516159339593</v>
       </c>
       <c r="I3" s="12">
-        <v>75.345440975642802</v>
+        <v>25.668998148625501</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1258,28 +1267,28 @@
         <v>19</v>
       </c>
       <c r="B4" s="12">
-        <v>3.3396268152061399</v>
+        <v>18.3175837846658</v>
       </c>
       <c r="C4" s="12">
-        <v>1.06522898396133</v>
+        <v>-0.23492748513700401</v>
       </c>
       <c r="D4" s="12">
-        <v>2.2913515460082099</v>
+        <v>3.4688807684054699</v>
       </c>
       <c r="E4" s="12">
-        <v>6.7293483232064002</v>
+        <v>-0.110433672218024</v>
       </c>
       <c r="F4" s="12">
-        <v>-0.210375231957283</v>
+        <v>0.44601697583396299</v>
       </c>
       <c r="G4" s="12">
-        <v>2.7673894114881299</v>
+        <v>2.4747501870125501</v>
       </c>
       <c r="H4" s="12">
-        <v>-3.2879506166974699</v>
+        <v>4.89015883298537</v>
       </c>
       <c r="I4" s="12">
-        <v>87.305380768784502</v>
+        <v>29.252029391548099</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1287,28 +1296,28 @@
         <v>21</v>
       </c>
       <c r="B5" s="12">
-        <v>5.4330505108965603</v>
+        <v>5.6531576035639599</v>
       </c>
       <c r="C5" s="12">
-        <v>-0.28100686998880903</v>
+        <v>-0.53423379121136905</v>
       </c>
       <c r="D5" s="12">
-        <v>0.165494611875838</v>
+        <v>2.0482386886328099</v>
       </c>
       <c r="E5" s="12">
-        <v>-0.40948826046377501</v>
+        <v>0.83786215452826796</v>
       </c>
       <c r="F5" s="12">
-        <v>-0.36637928818973298</v>
+        <v>-4.2222732805718997E-2</v>
       </c>
       <c r="G5" s="12">
-        <v>1.70622821583962</v>
+        <v>0.97298995307758496</v>
       </c>
       <c r="H5" s="12">
-        <v>9.1079511312440395</v>
+        <v>7.7896710820905399</v>
       </c>
       <c r="I5" s="12">
-        <v>84.644149948786307</v>
+        <v>16.7254629578761</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1316,28 +1325,28 @@
         <v>22</v>
       </c>
       <c r="B6" s="12">
-        <v>1.0392002254961701</v>
+        <v>-0.28330050835989601</v>
       </c>
       <c r="C6" s="12">
-        <v>0.84480128988587699</v>
+        <v>-0.37310196350531799</v>
       </c>
       <c r="D6" s="12">
-        <v>16.465481084219</v>
+        <v>14.065260405833399</v>
       </c>
       <c r="E6" s="12">
-        <v>-0.144698976403179</v>
+        <v>1.50983188274889E-2</v>
       </c>
       <c r="F6" s="12">
-        <v>7.75631428758801</v>
+        <v>7.2676093627985203</v>
       </c>
       <c r="G6" s="12">
-        <v>0.50366521496688599</v>
+        <v>-9.1516322383122795E-2</v>
       </c>
       <c r="H6" s="12">
-        <v>2.2250029703380001</v>
+        <v>3.0250587237817399</v>
       </c>
       <c r="I6" s="12">
-        <v>71.310233903909193</v>
+        <v>23.625108016992801</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1345,289 +1354,289 @@
         <v>23</v>
       </c>
       <c r="B7" s="12">
-        <v>6.2824138637025504</v>
+        <v>8.1623481671503892</v>
       </c>
       <c r="C7" s="12">
-        <v>0.74541518006422403</v>
+        <v>0.59708386848185102</v>
       </c>
       <c r="D7" s="12">
-        <v>-4.6160969394618698</v>
+        <v>2.5197164178323801</v>
       </c>
       <c r="E7" s="12">
-        <v>0.48586050517387402</v>
+        <v>-5.3304614445170997E-2</v>
       </c>
       <c r="F7" s="12">
-        <v>2.6073084105503499</v>
+        <v>3.7539996507070401</v>
       </c>
       <c r="G7" s="12">
-        <v>4.9132645695611199</v>
+        <v>1.8853871197713299</v>
       </c>
       <c r="H7" s="12">
-        <v>6.0019959337168496</v>
+        <v>8.4743164709671195</v>
       </c>
       <c r="I7" s="12">
-        <v>83.579838476692899</v>
+        <v>25.339547080465</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="B8" s="12">
-        <v>17.910148526701398</v>
+        <v>2.32914867780825</v>
       </c>
       <c r="C8" s="12">
-        <v>1.1083968276877101</v>
+        <v>2.1704985660260698</v>
       </c>
       <c r="D8" s="12">
-        <v>-1.79287926682863</v>
+        <v>12.2876934840915</v>
       </c>
       <c r="E8" s="12">
-        <v>0.81450770493332003</v>
+        <v>-0.21598679749668101</v>
       </c>
       <c r="F8" s="12">
-        <v>2.1348587332625999</v>
+        <v>-0.33034187736217202</v>
       </c>
       <c r="G8" s="12">
-        <v>0.38139458528203601</v>
+        <v>1.4842887075553799</v>
       </c>
       <c r="H8" s="12">
-        <v>5.7198704785400301</v>
+        <v>0.12933832053535499</v>
       </c>
       <c r="I8" s="12">
-        <v>73.723702410421495</v>
+        <v>17.8546390811577</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="12">
-        <v>8.8134219891704202</v>
+        <v>17.996553106037101</v>
       </c>
       <c r="C9" s="12">
-        <v>-0.64816652801144004</v>
+        <v>2.6489969221883398</v>
       </c>
       <c r="D9" s="12">
-        <v>13.5650399394255</v>
+        <v>1.10092575930186</v>
       </c>
       <c r="E9" s="12">
-        <v>0.49678318884715</v>
+        <v>1.71586158862074</v>
       </c>
       <c r="F9" s="12">
-        <v>1.5309802917134601</v>
+        <v>0.506950726227273</v>
       </c>
       <c r="G9" s="12">
-        <v>1.5205013533887799</v>
+        <v>0.86507684279073505</v>
       </c>
       <c r="H9" s="12">
-        <v>3.3323085194736302</v>
+        <v>5.4819464392910504</v>
       </c>
       <c r="I9" s="12">
-        <v>71.389131245992502</v>
+        <v>30.316311384457101</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="12">
-        <v>11.038929370899099</v>
+        <v>5.0628834331280599</v>
       </c>
       <c r="C10" s="12">
-        <v>-0.85952890366055601</v>
+        <v>-0.494828788032942</v>
       </c>
       <c r="D10" s="12">
-        <v>11.6399202863439</v>
+        <v>10.2707207876</v>
       </c>
       <c r="E10" s="12">
-        <v>-0.28622742826535102</v>
+        <v>-2.14452033336365E-2</v>
       </c>
       <c r="F10" s="12">
-        <v>8.6206279641520904</v>
+        <v>3.2083333122572202</v>
       </c>
       <c r="G10" s="12">
-        <v>0.94569056321130995</v>
+        <v>4.2200705283429603</v>
       </c>
       <c r="H10" s="12">
-        <v>8.8032911080238492</v>
+        <v>2.37671859970993</v>
       </c>
       <c r="I10" s="12">
-        <v>60.097297039295697</v>
+        <v>24.622452669671599</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B11" s="12">
-        <v>2.9560568124720499</v>
+        <v>10.922878127654499</v>
       </c>
       <c r="C11" s="12">
-        <v>-0.30230983747199203</v>
+        <v>-0.184351951166217</v>
       </c>
       <c r="D11" s="12">
-        <v>2.8574640970501601</v>
+        <v>8.6950838874448895</v>
       </c>
       <c r="E11" s="12">
-        <v>0.61435127672913004</v>
+        <v>4.2827795829147898E-2</v>
       </c>
       <c r="F11" s="12">
-        <v>8.0357152152810099E-2</v>
+        <v>6.0434644335314296</v>
       </c>
       <c r="G11" s="12">
-        <v>-0.13460052071433401</v>
+        <v>6.04059985123006</v>
       </c>
       <c r="H11" s="12">
-        <v>-7.8410889832669597E-2</v>
+        <v>9.0037947589202592</v>
       </c>
       <c r="I11" s="12">
-        <v>94.0070919096148</v>
+        <v>40.564296903444102</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B12" s="12">
-        <v>-1.22459924325595</v>
+        <v>5.3954231528796299</v>
       </c>
       <c r="C12" s="12">
-        <v>-2.7831533511508502</v>
+        <v>1.0276998621823401</v>
       </c>
       <c r="D12" s="12">
-        <v>-9.6946532652051491</v>
+        <v>11.3767914297049</v>
       </c>
       <c r="E12" s="12">
-        <v>0.45751856260178903</v>
+        <v>0.28270775475445198</v>
       </c>
       <c r="F12" s="12">
-        <v>2.49005024751736</v>
+        <v>5.1970003740020601E-2</v>
       </c>
       <c r="G12" s="12">
-        <v>4.7001081856666298</v>
+        <v>-1.94571412215897</v>
       </c>
       <c r="H12" s="12">
-        <v>1.0173591827091</v>
+        <v>-4.8556649679731799E-2</v>
       </c>
       <c r="I12" s="12">
-        <v>105.037369681117</v>
+        <v>16.140321431422599</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B13" s="12">
-        <v>4.73821131688333</v>
+        <v>9.8390305127144302</v>
       </c>
       <c r="C13" s="12">
-        <v>3.08013990558229</v>
+        <v>-0.19508849635523401</v>
       </c>
       <c r="D13" s="12">
-        <v>5.5685627267099402</v>
+        <v>4.4304486023623504</v>
       </c>
       <c r="E13" s="12">
-        <v>-4.1877386942900801</v>
+        <v>-0.203481747751977</v>
       </c>
       <c r="F13" s="12">
-        <v>0.91586705484203401</v>
+        <v>1.39205752077265</v>
       </c>
       <c r="G13" s="12">
-        <v>1.18335620101512</v>
+        <v>2.0551397505848699</v>
       </c>
       <c r="H13" s="12">
-        <v>-1.0001723039772601</v>
+        <v>3.8753640475609501</v>
       </c>
       <c r="I13" s="12">
-        <v>89.701773793234594</v>
+        <v>21.193470189888</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="12">
-        <v>6.6672555496199504</v>
+        <v>6.4223629879214599</v>
       </c>
       <c r="C14" s="12">
-        <v>0.804356685193652</v>
+        <v>3.3059495544532602</v>
       </c>
       <c r="D14" s="12">
-        <v>3.9971516577555501</v>
+        <v>9.3994861343993402E-2</v>
       </c>
       <c r="E14" s="12">
-        <v>-0.16136630994804099</v>
+        <v>3.1858863599641101</v>
       </c>
       <c r="F14" s="12">
-        <v>-6.9495546791320501E-2</v>
+        <v>9.1021237683968099</v>
       </c>
       <c r="G14" s="12">
-        <v>5.2245215960010896</v>
+        <v>-0.102820685603355</v>
       </c>
       <c r="H14" s="12">
-        <v>3.5804331170533801</v>
+        <v>5.1435221644416904</v>
       </c>
       <c r="I14" s="12">
-        <v>79.957143251115696</v>
+        <v>27.151019010917999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B15" s="12">
-        <v>11.561107195252699</v>
+        <v>11.993537520910699</v>
       </c>
       <c r="C15" s="12">
-        <v>2.2932814506523602</v>
+        <v>-7.0786613658013794E-2</v>
       </c>
       <c r="D15" s="12">
-        <v>-6.1303440583693199E-2</v>
+        <v>2.43827688536072</v>
       </c>
       <c r="E15" s="12">
-        <v>-0.18070355244274</v>
+        <v>1.68114876922978</v>
       </c>
       <c r="F15" s="12">
-        <v>10.519443105119599</v>
+        <v>0.21112242350201901</v>
       </c>
       <c r="G15" s="12">
-        <v>-4.8916245028243104</v>
+        <v>-0.12775341683554101</v>
       </c>
       <c r="H15" s="12">
-        <v>9.2658562907152504</v>
+        <v>0.30348742033621301</v>
       </c>
       <c r="I15" s="12">
-        <v>71.493943454110905</v>
+        <v>16.429032988845901</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B16" s="12">
-        <v>11.4343596042175</v>
+        <v>6.27537830819759</v>
       </c>
       <c r="C16" s="12">
-        <v>0.37079626074427702</v>
+        <v>-0.38889964834122298</v>
       </c>
       <c r="D16" s="12">
-        <v>3.0619872219749</v>
+        <v>2.9419662287769999</v>
       </c>
       <c r="E16" s="12">
-        <v>0.26278237492135498</v>
+        <v>0.92958520015324897</v>
       </c>
       <c r="F16" s="12">
-        <v>-1.52498309817262</v>
+        <v>0.26667406184161002</v>
       </c>
       <c r="G16" s="12">
-        <v>0.32221144128914397</v>
+        <v>-0.314390592488489</v>
       </c>
       <c r="H16" s="12">
-        <v>2.0129848248386</v>
+        <v>1.40511761377924</v>
       </c>
       <c r="I16" s="12">
-        <v>84.059861370186795</v>
+        <v>11.115431171919001</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1635,28 +1644,28 @@
         <v>28</v>
       </c>
       <c r="B17" s="12">
-        <v>2.2489799557933199</v>
+        <v>2.7184045668031298</v>
       </c>
       <c r="C17" s="12">
-        <v>2.0463138448605802</v>
+        <v>1.0658668418539901</v>
       </c>
       <c r="D17" s="12">
-        <v>12.3640502452019</v>
+        <v>15.4263957319412</v>
       </c>
       <c r="E17" s="12">
-        <v>0.36781546095963102</v>
+        <v>3.6630655774949501</v>
       </c>
       <c r="F17" s="12">
-        <v>1.5227937950844199</v>
+        <v>1.3087974097455799</v>
       </c>
       <c r="G17" s="12">
-        <v>3.7369799778971502</v>
+        <v>2.6370369221627801</v>
       </c>
       <c r="H17" s="12">
-        <v>14.154852752778901</v>
+        <v>12.189997446607199</v>
       </c>
       <c r="I17" s="12">
-        <v>63.558213967424102</v>
+        <v>39.009564496608803</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1664,87 +1673,68 @@
         <v>31</v>
       </c>
       <c r="B18" s="12">
-        <v>3.9548674716817098</v>
+        <v>6.6754002558993397</v>
       </c>
       <c r="C18" s="12">
-        <v>3.3094215991238101</v>
+        <v>-0.40502311558353599</v>
       </c>
       <c r="D18" s="12">
-        <v>4.5888724929466296</v>
+        <v>3.9899879317466702</v>
       </c>
       <c r="E18" s="12">
-        <v>5.1231559814727801</v>
+        <v>-0.43597558195234098</v>
       </c>
       <c r="F18" s="12">
-        <v>-2.3268816893273199</v>
+        <v>1.8053315785027099E-2</v>
       </c>
       <c r="G18" s="12">
-        <v>4.3812945467850097</v>
+        <v>1.74205193170928</v>
       </c>
       <c r="H18" s="12">
-        <v>0.304605872598118</v>
+        <v>5.7779746413663</v>
       </c>
       <c r="I18" s="12">
-        <v>80.664663724719304</v>
+        <v>17.362469378970701</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="12">
-        <v>1.55018273989375</v>
-      </c>
-      <c r="C19" s="12">
-        <v>1.9417504342040599</v>
-      </c>
-      <c r="D19" s="12">
-        <v>-1.95461849362608</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0.232766226269432</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.88341686931632202</v>
-      </c>
-      <c r="G19" s="12">
-        <v>0.51909796918715401</v>
-      </c>
-      <c r="H19" s="12">
-        <v>2.23186388402498</v>
-      </c>
-      <c r="I19" s="12">
-        <v>94.595540370730404</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="14">
-        <v>10.524136364312</v>
-      </c>
-      <c r="C20" s="14">
-        <v>-1.2615784287398499</v>
-      </c>
-      <c r="D20" s="14">
-        <v>10.4193855544587</v>
-      </c>
-      <c r="E20" s="14">
-        <v>-0.20139114680287601</v>
-      </c>
-      <c r="F20" s="14">
-        <v>3.2559715885348801</v>
-      </c>
-      <c r="G20" s="14">
-        <v>0.55165030886301603</v>
-      </c>
-      <c r="H20" s="14">
-        <v>6.0854995011881003</v>
-      </c>
-      <c r="I20" s="14">
-        <v>70.626326258185998</v>
-      </c>
+      <c r="B19" s="14">
+        <v>8.3899446607100394</v>
+      </c>
+      <c r="C19" s="14">
+        <v>-0.29767896789570902</v>
+      </c>
+      <c r="D19" s="14">
+        <v>8.4260201976761397</v>
+      </c>
+      <c r="E19" s="14">
+        <v>-7.6027606931805505E-2</v>
+      </c>
+      <c r="F19" s="14">
+        <v>4.7114112741346199</v>
+      </c>
+      <c r="G19" s="14">
+        <v>2.86020947080566</v>
+      </c>
+      <c r="H19" s="14">
+        <v>4.68412241053512</v>
+      </c>
+      <c r="I19" s="14">
+        <v>28.698001439034101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
@@ -1935,16 +1925,6 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1960,7 +1940,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1970,133 +1950,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
+      <c r="A1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="19" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="20" t="s">
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="20"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>58</v>
-      </c>
       <c r="P3" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="E4" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18">
         <v>13.813000994394899</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="22">
+      <c r="I4" s="17"/>
+      <c r="J4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="18">
         <v>7.3930744382742297</v>
       </c>
-      <c r="O4" s="21">
+      <c r="O4" s="17">
         <v>7</v>
       </c>
-      <c r="P4" s="22">
+      <c r="P4" s="18">
         <v>15.010234071807099</v>
       </c>
     </row>
@@ -2104,47 +2084,47 @@
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21" t="s">
+      <c r="B5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="18">
+        <v>4.7314987271284403</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="22">
-        <v>4.7314987271284403</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="N5" s="22">
+      <c r="N5" s="18">
         <v>6.9260625091699701</v>
       </c>
-      <c r="O5" s="21">
+      <c r="O5" s="17">
         <v>47</v>
       </c>
-      <c r="P5" s="22">
+      <c r="P5" s="18">
         <v>25.7500832051049</v>
       </c>
     </row>
@@ -2152,41 +2132,41 @@
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="18">
+        <v>14.5459147224738</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="22">
-        <v>14.5459147224738</v>
-      </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="22">
+      <c r="K6" s="17"/>
+      <c r="L6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18">
         <v>1.5476890131158301</v>
       </c>
-      <c r="O6" s="21">
+      <c r="O6" s="17">
         <v>48</v>
       </c>
-      <c r="P6" s="22">
+      <c r="P6" s="18">
         <v>32.472596635985802</v>
       </c>
     </row>
@@ -2194,49 +2174,49 @@
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="21" t="s">
+      <c r="B7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="18">
+        <v>21.9680592555085</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="22">
-        <v>21.9680592555085</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="22">
+      <c r="K7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="18">
         <v>43.397815716435701</v>
       </c>
-      <c r="O7" s="21">
+      <c r="O7" s="17">
         <v>44</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="18">
         <v>66.628412305160296</v>
       </c>
     </row>
@@ -2244,77 +2224,77 @@
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18">
+        <v>46.869703576928003</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22">
-        <v>46.869703576928003</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="22">
+      <c r="M8" s="17"/>
+      <c r="N8" s="18">
         <v>18.723486491219699</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="17">
         <v>29</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="18">
         <v>65.118829886833495</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22">
+        <v>41</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18">
         <v>50.902543885127599</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="22">
+      <c r="I9" s="17"/>
+      <c r="J9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18">
         <v>30.5730171973042</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="17">
         <v>2</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="18">
         <v>99.999998289872494</v>
       </c>
     </row>
@@ -2322,49 +2302,49 @@
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="22">
+      <c r="B10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="18">
         <v>7.2318882400686002</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="22">
+      <c r="I10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="18">
         <v>10.761138053583</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="17">
         <v>47</v>
       </c>
-      <c r="P10" s="22">
+      <c r="P10" s="18">
         <v>44.277304399635398</v>
       </c>
     </row>
@@ -2372,47 +2352,47 @@
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="22">
+      <c r="B11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="18">
         <v>13.0453089858563</v>
       </c>
-      <c r="I11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="N11" s="22">
+      <c r="I11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="N11" s="18">
         <v>13.180275148516399</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="17">
         <v>41</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="18">
         <v>32.027133493186298</v>
       </c>
     </row>
@@ -2420,47 +2400,47 @@
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="18">
+        <v>30.3027051145265</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="22">
-        <v>30.3027051145265</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M12" s="21"/>
-      <c r="N12" s="22">
+      <c r="L12" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18">
         <v>16.820689566885299</v>
       </c>
-      <c r="O12" s="21">
+      <c r="O12" s="17">
         <v>48</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="18">
         <v>61.150251021438599</v>
       </c>
     </row>
@@ -2468,87 +2448,87 @@
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="22">
+      <c r="B13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="18">
         <v>20.543576653187301</v>
       </c>
-      <c r="I13" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="21" t="s">
+      <c r="I13" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="N13" s="22">
+      <c r="J13" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" s="18">
         <v>37.865641231842197</v>
       </c>
-      <c r="O13" s="21">
+      <c r="O13" s="17">
         <v>40</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="18">
         <v>61.353189192038201</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22">
+        <v>42</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18">
         <v>99.999994948098703</v>
       </c>
-      <c r="I14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="M14" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="N14" s="22">
+      <c r="I14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" s="18">
         <v>26.648493516007399</v>
       </c>
-      <c r="O14" s="21">
+      <c r="O14" s="17">
         <v>2</v>
       </c>
-      <c r="P14" s="22">
+      <c r="P14" s="18">
         <v>97.5799616212676</v>
       </c>
     </row>
@@ -2556,45 +2536,45 @@
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22">
+      <c r="B15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18">
         <v>45.626916354184097</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="M15" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N15" s="22">
+      <c r="I15" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" s="18">
         <v>44.023978604520202</v>
       </c>
-      <c r="O15" s="21">
+      <c r="O15" s="17">
         <v>44</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="18">
         <v>70.204150781730704</v>
       </c>
     </row>
@@ -2602,45 +2582,45 @@
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="22">
+      <c r="F16" s="17"/>
+      <c r="G16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="18">
         <v>6.3640842062335601</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N16" s="22">
+      <c r="I16" s="17"/>
+      <c r="J16" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" s="18">
         <v>11.2665347659867</v>
       </c>
-      <c r="O16" s="21">
+      <c r="O16" s="17">
         <v>49</v>
       </c>
-      <c r="P16" s="22">
+      <c r="P16" s="18">
         <v>46.626418187891701</v>
       </c>
     </row>
@@ -2648,95 +2628,95 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="22">
+      <c r="B17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="18">
         <v>43.426424649990203</v>
       </c>
-      <c r="I17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="L17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="M17" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="N17" s="22">
+      <c r="I17" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N17" s="18">
         <v>41.570253763039901</v>
       </c>
-      <c r="O17" s="21">
+      <c r="O17" s="17">
         <v>37</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="18">
         <v>61.114729642958899</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="22">
+        <v>43</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="18">
         <v>1.8111201528302701</v>
       </c>
-      <c r="I18" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N18" s="22">
+      <c r="I18" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="18">
         <v>3.1391554467821199</v>
       </c>
-      <c r="O18" s="21">
+      <c r="O18" s="17">
         <v>45</v>
       </c>
-      <c r="P18" s="22">
+      <c r="P18" s="18">
         <v>24.250328135362601</v>
       </c>
     </row>
@@ -2744,49 +2724,49 @@
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="G19" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="H19" s="18">
+        <v>26.485517092593099</v>
+      </c>
+      <c r="I19" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="22">
-        <v>26.485517092593099</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L19" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M19" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N19" s="22">
+      <c r="J19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N19" s="18">
         <v>4.2849073811194698</v>
       </c>
-      <c r="O19" s="21">
+      <c r="O19" s="17">
         <v>52</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="18">
         <v>57.000252610546603</v>
       </c>
     </row>
@@ -2794,49 +2774,49 @@
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="22">
+      <c r="B20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="18">
         <v>34.844867065611297</v>
       </c>
-      <c r="I20" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N20" s="22">
+      <c r="I20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="18">
         <v>20.0522858049662</v>
       </c>
-      <c r="O20" s="21">
+      <c r="O20" s="17">
         <v>32</v>
       </c>
-      <c r="P20" s="22">
+      <c r="P20" s="18">
         <v>67.831021136782496</v>
       </c>
     </row>
@@ -2844,45 +2824,45 @@
       <c r="A21" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23" t="s">
+      <c r="B21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="20">
+        <v>5.9332010456594997</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="24">
-        <v>5.9332010456594997</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="M21" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="N21" s="24">
+      <c r="L21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" s="20">
         <v>14.5205420240063</v>
       </c>
-      <c r="O21" s="23">
+      <c r="O21" s="19">
         <v>44</v>
       </c>
-      <c r="P21" s="24">
+      <c r="P21" s="20">
         <v>32.641022257387398</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started working on text
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -598,9 +598,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -622,8 +619,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,7 +909,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection sqref="A1:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -919,13 +920,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1180,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1194,42 +1195,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="25" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1939,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1950,93 +1951,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="23" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="24" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="24"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="24" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2044,39 +2045,39 @@
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17">
         <v>13.813000994394899</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="18">
+      <c r="M4" s="16"/>
+      <c r="N4" s="17">
         <v>7.3930744382742297</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4" s="16">
         <v>7</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="17">
         <v>15.010234071807099</v>
       </c>
     </row>
@@ -2084,47 +2085,47 @@
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="18">
+      <c r="B5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="17">
         <v>4.7314987271284403</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M5" s="17" t="s">
+      <c r="I5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="17">
         <v>6.9260625091699701</v>
       </c>
-      <c r="O5" s="17">
+      <c r="O5" s="16">
         <v>47</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="17">
         <v>25.7500832051049</v>
       </c>
     </row>
@@ -2132,41 +2133,41 @@
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="18">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="17">
         <v>14.5459147224738</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17" t="s">
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="18">
+      <c r="K6" s="16"/>
+      <c r="L6" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="17">
         <v>1.5476890131158301</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6" s="16">
         <v>48</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="17">
         <v>32.472596635985802</v>
       </c>
     </row>
@@ -2174,49 +2175,49 @@
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="B7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="17">
         <v>21.9680592555085</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="K7" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="18">
+      <c r="K7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="17">
         <v>43.397815716435701</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="16">
         <v>44</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="17">
         <v>66.628412305160296</v>
       </c>
     </row>
@@ -2224,43 +2225,43 @@
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="B8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18">
+      <c r="G8" s="16"/>
+      <c r="H8" s="17">
         <v>46.869703576928003</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17" t="s">
+      <c r="I8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="17"/>
-      <c r="N8" s="18">
+      <c r="M8" s="16"/>
+      <c r="N8" s="17">
         <v>18.723486491219699</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="16">
         <v>29</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="17">
         <v>65.118829886833495</v>
       </c>
     </row>
@@ -2268,33 +2269,33 @@
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17">
         <v>50.902543885127599</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17" t="s">
+      <c r="I9" s="16"/>
+      <c r="J9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="18">
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="17">
         <v>30.5730171973042</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O9" s="16">
         <v>2</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="17">
         <v>99.999998289872494</v>
       </c>
     </row>
@@ -2302,49 +2303,49 @@
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="18">
+      <c r="B10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="17">
         <v>7.2318882400686002</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" s="17" t="s">
+      <c r="I10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="17">
         <v>10.761138053583</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O10" s="16">
         <v>47</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="17">
         <v>44.277304399635398</v>
       </c>
     </row>
@@ -2352,47 +2353,47 @@
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="18">
+      <c r="B11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="17">
         <v>13.0453089858563</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="17" t="s">
+      <c r="I11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M11" s="17" t="s">
+      <c r="L11" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="17">
         <v>13.180275148516399</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11" s="16">
         <v>41</v>
       </c>
-      <c r="P11" s="18">
+      <c r="P11" s="17">
         <v>32.027133493186298</v>
       </c>
     </row>
@@ -2400,47 +2401,47 @@
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="B12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="18">
+      <c r="F12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="17">
         <v>30.3027051145265</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K12" s="17" t="s">
+      <c r="I12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="L12" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M12" s="17"/>
-      <c r="N12" s="18">
+      <c r="L12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" s="16"/>
+      <c r="N12" s="17">
         <v>16.820689566885299</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12" s="16">
         <v>48</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="17">
         <v>61.150251021438599</v>
       </c>
     </row>
@@ -2448,45 +2449,45 @@
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="18">
+      <c r="B13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="17">
         <v>20.543576653187301</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="L13" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="N13" s="18">
+      <c r="K13" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" s="17">
         <v>37.865641231842197</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13" s="16">
         <v>40</v>
       </c>
-      <c r="P13" s="18">
+      <c r="P13" s="17">
         <v>61.353189192038201</v>
       </c>
     </row>
@@ -2494,41 +2495,41 @@
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18">
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17">
         <v>99.999994948098703</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="M14" s="17" t="s">
+      <c r="M14" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="N14" s="18">
+      <c r="N14" s="17">
         <v>26.648493516007399</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14" s="16">
         <v>2</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="17">
         <v>97.5799616212676</v>
       </c>
     </row>
@@ -2536,45 +2537,45 @@
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="17" t="s">
+      <c r="B15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18">
+      <c r="E15" s="16"/>
+      <c r="F15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17">
         <v>45.626916354184097</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L15" s="17" t="s">
+      <c r="J15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="M15" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N15" s="18">
+      <c r="M15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" s="17">
         <v>44.023978604520202</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15" s="16">
         <v>44</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P15" s="17">
         <v>70.204150781730704</v>
       </c>
     </row>
@@ -2582,45 +2583,45 @@
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="D16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="18">
+      <c r="F16" s="16"/>
+      <c r="G16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="17">
         <v>6.3640842062335601</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="K16" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N16" s="18">
+      <c r="K16" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" s="17">
         <v>11.2665347659867</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="16">
         <v>49</v>
       </c>
-      <c r="P16" s="18">
+      <c r="P16" s="17">
         <v>46.626418187891701</v>
       </c>
     </row>
@@ -2628,47 +2629,47 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17" t="s">
+      <c r="B17" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="17">
         <v>43.426424649990203</v>
       </c>
-      <c r="I17" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="N17" s="18">
+      <c r="I17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N17" s="17">
         <v>41.570253763039901</v>
       </c>
-      <c r="O17" s="17">
+      <c r="O17" s="16">
         <v>37</v>
       </c>
-      <c r="P17" s="18">
+      <c r="P17" s="17">
         <v>61.114729642958899</v>
       </c>
     </row>
@@ -2676,47 +2677,47 @@
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="17" t="s">
+      <c r="B18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="18">
+      <c r="E18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="17">
         <v>1.8111201528302701</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J18" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L18" s="17" t="s">
+      <c r="J18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="M18" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N18" s="18">
+      <c r="M18" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="17">
         <v>3.1391554467821199</v>
       </c>
-      <c r="O18" s="17">
+      <c r="O18" s="16">
         <v>45</v>
       </c>
-      <c r="P18" s="18">
+      <c r="P18" s="17">
         <v>24.250328135362601</v>
       </c>
     </row>
@@ -2724,49 +2725,49 @@
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="B19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="17">
         <v>26.485517092593099</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K19" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N19" s="18">
+      <c r="K19" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N19" s="17">
         <v>4.2849073811194698</v>
       </c>
-      <c r="O19" s="17">
+      <c r="O19" s="16">
         <v>52</v>
       </c>
-      <c r="P19" s="18">
+      <c r="P19" s="17">
         <v>57.000252610546603</v>
       </c>
     </row>
@@ -2774,49 +2775,49 @@
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H20" s="18">
+      <c r="B20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="17">
         <v>34.844867065611297</v>
       </c>
-      <c r="I20" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" s="17" t="s">
+      <c r="I20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K20" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N20" s="18">
+      <c r="K20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="17">
         <v>20.0522858049662</v>
       </c>
-      <c r="O20" s="17">
+      <c r="O20" s="16">
         <v>32</v>
       </c>
-      <c r="P20" s="18">
+      <c r="P20" s="17">
         <v>67.831021136782496</v>
       </c>
     </row>
@@ -2824,45 +2825,45 @@
       <c r="A21" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="19" t="s">
+      <c r="D21" s="18"/>
+      <c r="E21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="20">
+      <c r="G21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="19">
         <v>5.9332010456594997</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19" t="s">
+      <c r="I21" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="L21" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="N21" s="20">
+      <c r="L21" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" s="19">
         <v>14.5205420240063</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="18">
         <v>44</v>
       </c>
-      <c r="P21" s="20">
+      <c r="P21" s="19">
         <v>32.641022257387398</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first section of results done
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -610,6 +610,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -622,10 +626,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,13 +922,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1181,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1195,42 +1197,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="21" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1293,7 +1295,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="12">
@@ -1322,7 +1324,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="12">
@@ -1351,7 +1353,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="12">
@@ -1380,7 +1382,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="12">
@@ -1409,7 +1411,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="12">
@@ -1438,7 +1440,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="12">
@@ -1467,7 +1469,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="12">
@@ -1496,7 +1498,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="26" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="12">
@@ -1525,7 +1527,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="12">
@@ -1554,7 +1556,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="26" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="12">
@@ -1583,7 +1585,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="12">
@@ -1612,7 +1614,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="26" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="12">
@@ -1641,7 +1643,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="12">
@@ -1670,7 +1672,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="26" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="12">
@@ -1699,7 +1701,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="14">
@@ -1940,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1951,93 +1953,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="21" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="23" t="s">
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="23"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2130,7 +2132,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -2172,7 +2174,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -2222,7 +2224,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -2266,7 +2268,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="26" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="16"/>
@@ -2300,7 +2302,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -2350,7 +2352,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -2398,7 +2400,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -2446,7 +2448,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -2492,7 +2494,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="16" t="s">
@@ -2534,7 +2536,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -2580,7 +2582,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -2626,7 +2628,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="26" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="16" t="s">
@@ -2674,7 +2676,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B18" s="16" t="s">
@@ -2722,7 +2724,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="26" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
@@ -2772,7 +2774,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -2822,7 +2824,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="18" t="s">

</xml_diff>

<commit_message>
second section of results done
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -357,46 +357,6 @@
   </si>
   <si>
     <t>**+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>Table 3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Significant explanatory variables (i.e. local, climate and space variables) demonstrated by forward and backward selection based on AIC. Direction of the effect is indicated by + and − symbols.  Empty space means that the variable was not selected for the response. For spatial variables, only the number of selected significant eigenvectors is shown. Explaied deviance (%) indicates how much the model explains the dependent variable based on adjusted R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>. ***: p ≤ 0.0001, **: p ≤ 0.001, *: p≤ 0.05, ns: p &gt; 0.05.</t>
-    </r>
   </si>
   <si>
     <t>P. foliosus</t>
@@ -460,6 +420,27 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> (Peres-Neto et al. 2006) from partial redundancy analysis, partial least squares, and generalized linear models.  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>Table 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Significant explanatory variables (i.e. local, climate and space variables) demonstrated by selection techniques.  Values are from individual models by category as input to variation partitioning analyses.  Direction of the effect is indicated by + and – symbols from the selected regression model, excluding results for assemblage composition that used forward selection by permutation.  Empty space means that the variable was not selected for the response. For spatial variables, only the number of selected significant eigenvectors is shown. Explained deviance (%) indicates how much the model explains the dependent variable based on adjusted R2 and does not consider joint effects with the remaining categories (see Table 2). ***: p ≤ 0.0001, **: p ≤ 0.001, *: p≤ 0.05, ns: p &gt; 0.05.</t>
     </r>
   </si>
 </sst>
@@ -1183,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
@@ -1198,7 +1179,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1233,7 +1214,7 @@
         <v>34</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1383,7 +1364,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="12">
         <v>2.32914867780825</v>
@@ -1499,7 +1480,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="12">
         <v>5.3954231528796299</v>
@@ -1615,7 +1596,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="12">
         <v>6.27537830819759</v>
@@ -1942,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1952,9 +1933,9 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>

</xml_diff>

<commit_message>
figs/tabs updated for new results
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="67">
   <si>
     <t>Secchi depth (m)</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>P. friesii</t>
-  </si>
-  <si>
     <t>P. strictifolius</t>
   </si>
   <si>
@@ -399,6 +396,15 @@
     </r>
   </si>
   <si>
+    <t>**+</t>
+  </si>
+  <si>
+    <t>*-</t>
+  </si>
+  <si>
+    <t>**-</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -416,7 +422,26 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> Significant explanatory variables (i.e. local, climate and space variables) demonstrated by selection techniques.  Values are from individual models by category as input to variation partitioning analyses.  Direction of the effect is indicated by + and – symbols from the selected regression model, excluding results for assemblage composition that modelled mutiple response variables with redundancy analysis.  Empty space means that the variable was not selected for the response. For spatial variables, only the number of selected significant eigenvectors is shown. Explained variance (%) indicates how much the model explains the dependent variable based on adjusted R2 and does not consider joint effects with the remaining categories (see Table 2). ***: p ≤ 0.0001, **: p ≤ 0.001, *: p≤ 0.05.</t>
+      <t xml:space="preserve"> Significant explanatory variables (i.e. local, climate and space variables) demonstrated by selection techniques.  Values are from individual models by category as input to variation partitioning analyses.  Direction of the effect is indicated by + and – symbols from the selected regression model, excluding results for assemblage composition that modelled mutiple species with redundancy analysis.  Empty space means that the variable was not selected for the response. For spatial variables, only the number of selected significant eigenvectors is shown. Explained variance (%) indicates how much the model explains the dependent variable based on adjusted R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and does not consider joint effects with the remaining categories (see Table 2). ***: p ≤ 0.0001, **: p ≤ 0.001, *: p≤ 0.05.</t>
     </r>
   </si>
 </sst>
@@ -487,7 +512,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -515,11 +540,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -563,12 +597,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -581,7 +610,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,13 +916,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1135,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1156,17 +1196,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="A1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
@@ -1196,556 +1236,540 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="12">
-        <v>4.1700931015078098</v>
-      </c>
-      <c r="C3" s="12">
-        <v>0.89084916919189805</v>
-      </c>
-      <c r="D3" s="12">
-        <v>7.6305556797126002</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0.41452351773674201</v>
-      </c>
-      <c r="F3" s="12">
-        <v>5.7322177299597703</v>
-      </c>
-      <c r="G3" s="12">
-        <v>3.4091403891849699</v>
-      </c>
-      <c r="H3" s="12">
-        <v>11.2645406257971</v>
-      </c>
-      <c r="I3" s="12">
-        <v>33.511920213090903</v>
+      <c r="B3" s="28">
+        <v>3.8259046021258598</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0.63218151361807995</v>
+      </c>
+      <c r="D3" s="28">
+        <v>6.6330984986780397</v>
+      </c>
+      <c r="E3" s="28">
+        <v>0.33220179258222099</v>
+      </c>
+      <c r="F3" s="28">
+        <v>6.1657584622845398</v>
+      </c>
+      <c r="G3" s="28">
+        <v>3.38036039408495</v>
+      </c>
+      <c r="H3" s="28">
+        <v>11.844547267379699</v>
+      </c>
+      <c r="I3" s="28">
+        <v>32.814052530753401</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="12">
-        <v>18.421684773159399</v>
-      </c>
-      <c r="C4" s="12">
-        <v>-0.23290558580322299</v>
-      </c>
-      <c r="D4" s="12">
-        <v>2.1751209107256702</v>
-      </c>
-      <c r="E4" s="12">
-        <v>-0.15014411440063</v>
-      </c>
-      <c r="F4" s="12">
-        <v>0.443995076500181</v>
-      </c>
-      <c r="G4" s="12">
-        <v>2.37064919851893</v>
-      </c>
-      <c r="H4" s="12">
-        <v>4.92986927516798</v>
-      </c>
-      <c r="I4" s="12">
-        <v>27.9582695338683</v>
+      <c r="B4" s="29">
+        <v>11.528157280018499</v>
+      </c>
+      <c r="C4" s="29">
+        <v>-0.39906133671750998</v>
+      </c>
+      <c r="D4" s="29">
+        <v>13.7694529306793</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.108096301396055</v>
+      </c>
+      <c r="F4" s="29">
+        <v>5.3057407524357396</v>
+      </c>
+      <c r="G4" s="29">
+        <v>3.9764452332559399</v>
+      </c>
+      <c r="H4" s="29">
+        <v>11.526329083953501</v>
+      </c>
+      <c r="I4" s="29">
+        <v>45.815160245021602</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="12">
-        <v>4.2947268871176902</v>
-      </c>
-      <c r="C5" s="12">
-        <v>0.140386577368357</v>
-      </c>
-      <c r="D5" s="12">
-        <v>3.31808631343206</v>
-      </c>
-      <c r="E5" s="12">
-        <v>-0.54680577482190096</v>
-      </c>
-      <c r="F5" s="12">
-        <v>-0.33785788069134998</v>
-      </c>
-      <c r="G5" s="12">
-        <v>3.93111429358868</v>
-      </c>
-      <c r="H5" s="12">
-        <v>7.5746453873758899</v>
-      </c>
-      <c r="I5" s="12">
-        <v>18.374295803369399</v>
+      <c r="B5" s="29">
+        <v>3.67524595560204</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.63619684933756704</v>
+      </c>
+      <c r="D5" s="29">
+        <v>3.2920969463023102</v>
+      </c>
+      <c r="E5" s="29">
+        <v>2.7172877415922301</v>
+      </c>
+      <c r="F5" s="29">
+        <v>1.99585595306025</v>
+      </c>
+      <c r="G5" s="29">
+        <v>2.8958174207390202</v>
+      </c>
+      <c r="H5" s="29">
+        <v>21.152809828810199</v>
+      </c>
+      <c r="I5" s="29">
+        <v>36.365310695443597</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="12">
-        <v>-0.34628502072289202</v>
-      </c>
-      <c r="C6" s="12">
-        <v>-9.9914864234818004E-2</v>
-      </c>
-      <c r="D6" s="12">
-        <v>17.980794947730999</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1.5867333700214599E-2</v>
-      </c>
-      <c r="F6" s="12">
-        <v>6.99442226352802</v>
-      </c>
-      <c r="G6" s="12">
-        <v>-2.8531810020127099E-2</v>
-      </c>
-      <c r="H6" s="12">
-        <v>3.0242897089090102</v>
-      </c>
-      <c r="I6" s="12">
-        <v>27.5406425588905</v>
+      <c r="B6" s="29">
+        <v>2.3372047737642601</v>
+      </c>
+      <c r="C6" s="29">
+        <v>-8.7018648078196495E-2</v>
+      </c>
+      <c r="D6" s="29">
+        <v>20.016525895666199</v>
+      </c>
+      <c r="E6" s="29">
+        <v>0.68552936784267404</v>
+      </c>
+      <c r="F6" s="29">
+        <v>9.3019492673961608</v>
+      </c>
+      <c r="G6" s="29">
+        <v>-0.84031338205338102</v>
+      </c>
+      <c r="H6" s="29">
+        <v>15.933595068944101</v>
+      </c>
+      <c r="I6" s="29">
+        <v>47.347472343481797</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="12">
-        <v>5.8536073126550301</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0.80136177096165095</v>
-      </c>
-      <c r="D7" s="12">
-        <v>4.2634723663647502</v>
-      </c>
-      <c r="E7" s="12">
-        <v>3.2151343830477699E-2</v>
-      </c>
-      <c r="F7" s="12">
-        <v>3.5497217482272401</v>
-      </c>
-      <c r="G7" s="12">
-        <v>4.1941279742666904</v>
-      </c>
-      <c r="H7" s="12">
-        <v>8.3888605126914797</v>
-      </c>
-      <c r="I7" s="12">
-        <v>27.0833030289973</v>
+      <c r="B7" s="29">
+        <v>0.98940903130942903</v>
+      </c>
+      <c r="C7" s="29">
+        <v>2.2247251257090799</v>
+      </c>
+      <c r="D7" s="29">
+        <v>3.0884995219489801</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0.36944645829869399</v>
+      </c>
+      <c r="F7" s="29">
+        <v>1.74622977596202</v>
+      </c>
+      <c r="G7" s="29">
+        <v>5.4803350191714602</v>
+      </c>
+      <c r="H7" s="29">
+        <v>14.326338386109301</v>
+      </c>
+      <c r="I7" s="29">
+        <v>28.224983318509</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="12">
-        <v>2.32914867780825</v>
-      </c>
-      <c r="C8" s="12">
-        <v>2.1704985660260698</v>
-      </c>
-      <c r="D8" s="12">
-        <v>12.2876934840915</v>
-      </c>
-      <c r="E8" s="12">
-        <v>-0.21598679749668101</v>
-      </c>
-      <c r="F8" s="12">
-        <v>-0.33034187736217202</v>
-      </c>
-      <c r="G8" s="12">
-        <v>1.4842887075553799</v>
-      </c>
-      <c r="H8" s="12">
-        <v>0.12933832053535499</v>
-      </c>
-      <c r="I8" s="12">
-        <v>17.8546390811577</v>
+      <c r="B8" s="29">
+        <v>7.7116585255798703E-2</v>
+      </c>
+      <c r="C8" s="29">
+        <v>2.0930214857060299</v>
+      </c>
+      <c r="D8" s="29">
+        <v>7.6929038157176102</v>
+      </c>
+      <c r="E8" s="29">
+        <v>-0.28718401809252297</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1.75040083001413</v>
+      </c>
+      <c r="G8" s="29">
+        <v>-0.49583382154171401</v>
+      </c>
+      <c r="H8" s="29">
+        <v>2.2617546388469401</v>
+      </c>
+      <c r="I8" s="29">
+        <v>13.092179515906301</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="29">
+        <v>13.981264010342599</v>
+      </c>
+      <c r="C9" s="29">
+        <v>0.35003000383149202</v>
+      </c>
+      <c r="D9" s="29">
+        <v>7.5918874075822096</v>
+      </c>
+      <c r="E9" s="29">
+        <v>1.86981289264796</v>
+      </c>
+      <c r="F9" s="29">
+        <v>3.9465835372886602</v>
+      </c>
+      <c r="G9" s="29">
+        <v>2.2492551053376899</v>
+      </c>
+      <c r="H9" s="29">
+        <v>5.9244874817844702</v>
+      </c>
+      <c r="I9" s="29">
+        <v>35.913320438814999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="29">
+        <v>12.022892934780399</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0.85018854770078101</v>
+      </c>
+      <c r="D10" s="29">
+        <v>10.2667558804467</v>
+      </c>
+      <c r="E10" s="29">
+        <v>-0.78072047573788395</v>
+      </c>
+      <c r="F10" s="29">
+        <v>4.0067158531511398</v>
+      </c>
+      <c r="G10" s="29">
+        <v>10.2985022973547</v>
+      </c>
+      <c r="H10" s="29">
+        <v>6.1469262136083698</v>
+      </c>
+      <c r="I10" s="29">
+        <v>42.811261251304202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="29">
+        <v>4.0312116339573798</v>
+      </c>
+      <c r="C11" s="29">
+        <v>-0.32605531797234</v>
+      </c>
+      <c r="D11" s="29">
+        <v>7.2822142948131701</v>
+      </c>
+      <c r="E11" s="29">
+        <v>-3.7973580591921199E-2</v>
+      </c>
+      <c r="F11" s="29">
+        <v>4.6338970274099198</v>
+      </c>
+      <c r="G11" s="29">
+        <v>1.38152650403249</v>
+      </c>
+      <c r="H11" s="29">
+        <v>5.4051075435308498</v>
+      </c>
+      <c r="I11" s="29">
+        <v>22.3699281051795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="29">
+        <v>5.86416232548794</v>
+      </c>
+      <c r="C12" s="29">
+        <v>-0.15893741171891801</v>
+      </c>
+      <c r="D12" s="29">
+        <v>13.0006647662969</v>
+      </c>
+      <c r="E12" s="29">
+        <v>0.16932059242872299</v>
+      </c>
+      <c r="F12" s="29">
+        <v>0.66963028565191196</v>
+      </c>
+      <c r="G12" s="29">
+        <v>19.1135099552871</v>
+      </c>
+      <c r="H12" s="29">
+        <v>29.1973682696031</v>
+      </c>
+      <c r="I12" s="29">
+        <v>67.855718783036707</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1.8516155304474899</v>
+      </c>
+      <c r="C13" s="29">
+        <v>-0.30751293607740299</v>
+      </c>
+      <c r="D13" s="29">
+        <v>17.146871713932899</v>
+      </c>
+      <c r="E13" s="29">
+        <v>-1.0499248374495901E-2</v>
+      </c>
+      <c r="F13" s="29">
+        <v>4.6484270904603902</v>
+      </c>
+      <c r="G13" s="29">
+        <v>5.8636338276242803</v>
+      </c>
+      <c r="H13" s="29">
+        <v>2.8932272268313199</v>
+      </c>
+      <c r="I13" s="29">
+        <v>32.085763204844497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="29">
+        <v>-3.7712740313389198E-2</v>
+      </c>
+      <c r="C14" s="29">
+        <v>0.97570126684389802</v>
+      </c>
+      <c r="D14" s="29">
+        <v>8.1552200772493997</v>
+      </c>
+      <c r="E14" s="29">
+        <v>8.50590770211435E-2</v>
+      </c>
+      <c r="F14" s="29">
+        <v>15.5469863625242</v>
+      </c>
+      <c r="G14" s="29">
+        <v>3.6290714800138799</v>
+      </c>
+      <c r="H14" s="29">
+        <v>19.793442652207599</v>
+      </c>
+      <c r="I14" s="29">
+        <v>48.147768175546702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="29">
+        <v>4.6418657411277504</v>
+      </c>
+      <c r="C15" s="29">
+        <v>0.45480373995631102</v>
+      </c>
+      <c r="D15" s="29">
+        <v>5.7999705323769204</v>
+      </c>
+      <c r="E15" s="29">
+        <v>0.58691838065637603</v>
+      </c>
+      <c r="F15" s="29">
+        <v>1.11239611070338</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0.63419021899022698</v>
+      </c>
+      <c r="H15" s="29">
+        <v>1.69282181314772</v>
+      </c>
+      <c r="I15" s="29">
+        <v>14.9229665369587</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="29">
+        <v>8.2489420956514206</v>
+      </c>
+      <c r="C16" s="29">
+        <v>0.10002970178533099</v>
+      </c>
+      <c r="D16" s="29">
+        <v>12.0963518683893</v>
+      </c>
+      <c r="E16" s="29">
+        <v>-0.41700196504258502</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0.99205307178151803</v>
+      </c>
+      <c r="G16" s="29">
+        <v>3.94003644893575</v>
+      </c>
+      <c r="H16" s="29">
+        <v>16.620361696458801</v>
+      </c>
+      <c r="I16" s="29">
+        <v>41.5807729179596</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="29">
+        <v>2.0372848390243399</v>
+      </c>
+      <c r="C17" s="29">
+        <v>0.286527114234159</v>
+      </c>
+      <c r="D17" s="29">
+        <v>7.3159369089321498</v>
+      </c>
+      <c r="E17" s="29">
+        <v>0.28891363718901403</v>
+      </c>
+      <c r="F17" s="29">
+        <v>6.1746497224714796</v>
+      </c>
+      <c r="G17" s="29">
+        <v>3.19368953885746</v>
+      </c>
+      <c r="H17" s="29">
+        <v>8.6159278006584508</v>
+      </c>
+      <c r="I17" s="29">
+        <v>27.9129295613671</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="12">
-        <v>2.3717262362234699</v>
-      </c>
-      <c r="C9" s="12">
-        <v>0.39120488672301801</v>
-      </c>
-      <c r="D9" s="12">
-        <v>6.1374833598443104</v>
-      </c>
-      <c r="E9" s="12">
-        <v>-0.25697313450017101</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0.22649738382984899</v>
-      </c>
-      <c r="G9" s="12">
-        <v>1.32623672112573</v>
-      </c>
-      <c r="H9" s="12">
-        <v>1.5866301106770799</v>
-      </c>
-      <c r="I9" s="12">
-        <v>11.782805563923301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="12">
-        <v>16.219026845344001</v>
-      </c>
-      <c r="C10" s="12">
-        <v>-0.31550083928876299</v>
-      </c>
-      <c r="D10" s="12">
-        <v>3.35794392798981</v>
-      </c>
-      <c r="E10" s="12">
-        <v>-3.0387189408009899E-2</v>
-      </c>
-      <c r="F10" s="12">
-        <v>1.9563582911466599</v>
-      </c>
-      <c r="G10" s="12">
-        <v>2.28921064246344</v>
-      </c>
-      <c r="H10" s="12">
-        <v>7.5815876783401697</v>
-      </c>
-      <c r="I10" s="12">
-        <v>31.058239356587301</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="12">
-        <v>4.3633995786431701</v>
-      </c>
-      <c r="C11" s="12">
-        <v>-0.48569124007611397</v>
-      </c>
-      <c r="D11" s="12">
-        <v>12.462740719037299</v>
-      </c>
-      <c r="E11" s="12">
-        <v>0.27468341363702198</v>
-      </c>
-      <c r="F11" s="12">
-        <v>3.1991957643003901</v>
-      </c>
-      <c r="G11" s="12">
-        <v>4.9195543828278501</v>
-      </c>
-      <c r="H11" s="12">
-        <v>2.0805899827392702</v>
-      </c>
-      <c r="I11" s="12">
-        <v>26.8144726011088</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="12">
-        <v>11.037321903138199</v>
-      </c>
-      <c r="C12" s="12">
-        <v>-0.135432719838946</v>
-      </c>
-      <c r="D12" s="12">
-        <v>9.8216057049024705</v>
-      </c>
-      <c r="E12" s="12">
-        <v>5.4502323717664503E-2</v>
-      </c>
-      <c r="F12" s="12">
-        <v>5.9945452022041597</v>
-      </c>
-      <c r="G12" s="12">
-        <v>5.9261560757463503</v>
-      </c>
-      <c r="H12" s="12">
-        <v>8.9921202310317394</v>
-      </c>
-      <c r="I12" s="12">
-        <v>41.690818720901603</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="12">
-        <v>3.0930470283215299</v>
-      </c>
-      <c r="C13" s="12">
-        <v>0.61245366575562998</v>
-      </c>
-      <c r="D13" s="12">
-        <v>14.036261697817</v>
-      </c>
-      <c r="E13" s="12">
-        <v>3.3297201204756899</v>
-      </c>
-      <c r="F13" s="12">
-        <v>1.7622105858439401</v>
-      </c>
-      <c r="G13" s="12">
-        <v>2.2623944606443902</v>
-      </c>
-      <c r="H13" s="12">
-        <v>12.5233429036264</v>
-      </c>
-      <c r="I13" s="12">
-        <v>37.619430462484601</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="12">
-        <v>7.8547847864926501</v>
-      </c>
-      <c r="C14" s="12">
-        <v>0.26200553693872503</v>
-      </c>
-      <c r="D14" s="12">
-        <v>11.755733009214801</v>
-      </c>
-      <c r="E14" s="12">
-        <v>-0.39586586647025701</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0.93496348747869096</v>
-      </c>
-      <c r="G14" s="12">
-        <v>4.0393854768066504</v>
-      </c>
-      <c r="H14" s="12">
-        <v>4.0677481662792303</v>
-      </c>
-      <c r="I14" s="12">
-        <v>28.5187545967405</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="12">
-        <v>7.2716819971721796</v>
-      </c>
-      <c r="C15" s="12">
-        <v>1.2122233521655299</v>
-      </c>
-      <c r="D15" s="12">
-        <v>0.69323326539660901</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0.116261414903684</v>
-      </c>
-      <c r="F15" s="12">
-        <v>10.680822127404999</v>
-      </c>
-      <c r="G15" s="12">
-        <v>-6.3165805731735206E-2</v>
-      </c>
-      <c r="H15" s="12">
-        <v>8.7281749527816199</v>
-      </c>
-      <c r="I15" s="12">
-        <v>28.639231304092899</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="12">
-        <v>10.3612893084838</v>
-      </c>
-      <c r="C16" s="12">
-        <v>-0.15133951073146301</v>
-      </c>
-      <c r="D16" s="12">
-        <v>8.5017539268799993</v>
-      </c>
-      <c r="E16" s="12">
-        <v>1.3442960135611</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0.29167532057546902</v>
-      </c>
-      <c r="G16" s="12">
-        <v>1.5044947955914001</v>
-      </c>
-      <c r="H16" s="12">
-        <v>0.64034017600489401</v>
-      </c>
-      <c r="I16" s="12">
-        <v>22.492510030365199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="12">
-        <v>5.2718159184874196</v>
-      </c>
-      <c r="C17" s="12">
-        <v>0.870265697389905</v>
-      </c>
-      <c r="D17" s="12">
-        <v>9.5963717089703806</v>
-      </c>
-      <c r="E17" s="12">
-        <v>-0.96629210911368701</v>
-      </c>
-      <c r="F17" s="12">
-        <v>-1.2572354971884101</v>
-      </c>
-      <c r="G17" s="12">
-        <v>3.1456362691212001</v>
-      </c>
-      <c r="H17" s="12">
-        <v>6.3082911685276502</v>
-      </c>
-      <c r="I17" s="12">
-        <v>22.968853156194399</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="12">
-        <v>5.6434405033882404</v>
-      </c>
-      <c r="C18" s="12">
-        <v>-0.18871622527996099</v>
-      </c>
-      <c r="D18" s="12">
-        <v>5.90409208997671</v>
-      </c>
-      <c r="E18" s="12">
-        <v>-0.23069524686187801</v>
-      </c>
-      <c r="F18" s="12">
-        <v>6.6490638780347694E-2</v>
-      </c>
-      <c r="G18" s="12">
-        <v>0.31754721232085698</v>
-      </c>
-      <c r="H18" s="12">
-        <v>2.56539806079437</v>
-      </c>
-      <c r="I18" s="12">
-        <v>14.077557033118699</v>
+      <c r="B18" s="29">
+        <v>-0.29360900539779899</v>
+      </c>
+      <c r="C18" s="29">
+        <v>0.72891679040278901</v>
+      </c>
+      <c r="D18" s="29">
+        <v>0.41902386699275201</v>
+      </c>
+      <c r="E18" s="29">
+        <v>0.122246570823836</v>
+      </c>
+      <c r="F18" s="29">
+        <v>5.1835460768454498</v>
+      </c>
+      <c r="G18" s="29">
+        <v>0.37006346428718501</v>
+      </c>
+      <c r="H18" s="29">
+        <v>5.6365160823393996</v>
+      </c>
+      <c r="I18" s="29">
+        <v>12.166703846293601</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="12">
-        <v>-0.117331600077697</v>
-      </c>
-      <c r="C19" s="12">
-        <v>0.60149269931387706</v>
-      </c>
-      <c r="D19" s="12">
-        <v>2.86793753600797</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0.18582043707604501</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0.88474910806682905</v>
-      </c>
-      <c r="G19" s="12">
-        <v>0.52347986748828601</v>
-      </c>
-      <c r="H19" s="12">
-        <v>2.9565574918596198</v>
-      </c>
-      <c r="I19" s="12">
-        <v>7.9027055397349297</v>
+      <c r="A19" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="14">
+        <v>0.14655107668312101</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0.43201004064258303</v>
+      </c>
+      <c r="D19" s="14">
+        <v>5.3823753575645004</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.42279392187943898</v>
+      </c>
+      <c r="F19" s="14">
+        <v>9.9694750877389993</v>
+      </c>
+      <c r="G19" s="14">
+        <v>0.46877663952258303</v>
+      </c>
+      <c r="H19" s="14">
+        <v>2.7947977504978301</v>
+      </c>
+      <c r="I19" s="14">
+        <v>19.616779874529101</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="14">
-        <v>8.3052469573594205</v>
-      </c>
-      <c r="C20" s="14">
-        <v>-0.25915661704076798</v>
-      </c>
-      <c r="D20" s="14">
-        <v>12.9640155988139</v>
-      </c>
-      <c r="E20" s="14">
-        <v>-9.9188334592770197E-2</v>
-      </c>
-      <c r="F20" s="14">
-        <v>3.5547429290164101</v>
-      </c>
-      <c r="G20" s="14">
-        <v>3.1126971543941502</v>
-      </c>
-      <c r="H20" s="14">
-        <v>5.8254291324593597</v>
-      </c>
-      <c r="I20" s="14">
-        <v>33.403786820409799</v>
+      <c r="B20" s="21">
+        <f>AVERAGE(B5:B19)</f>
+        <v>3.9715629858481858</v>
+      </c>
+      <c r="C20" s="21">
+        <f t="shared" ref="C20:I20" si="0">AVERAGE(C5:C19)</f>
+        <v>0.55017509015354427</v>
+      </c>
+      <c r="D20" s="21">
+        <f t="shared" si="0"/>
+        <v>8.5698199236141317</v>
+      </c>
+      <c r="E20" s="21">
+        <f t="shared" si="0"/>
+        <v>0.38559662350271195</v>
+      </c>
+      <c r="F20" s="21">
+        <f t="shared" si="0"/>
+        <v>4.7785864034973065</v>
+      </c>
+      <c r="G20" s="21">
+        <f t="shared" si="0"/>
+        <v>3.8788173811039157</v>
+      </c>
+      <c r="H20" s="21">
+        <f t="shared" si="0"/>
+        <v>10.559698830225228</v>
+      </c>
+      <c r="I20" s="21">
+        <f t="shared" si="0"/>
+        <v>32.694257237945031</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="27">
-        <f>AVERAGE(B5:B20)</f>
-        <v>5.8629154574896534</v>
-      </c>
-      <c r="C21" s="27">
-        <f t="shared" ref="C21:D21" si="0">AVERAGE(C5:C20)</f>
-        <v>0.33913379600949567</v>
-      </c>
-      <c r="D21" s="27">
-        <f t="shared" si="0"/>
-        <v>8.4968262285294109</v>
-      </c>
-      <c r="E21" s="27">
-        <f>AVERAGE(E5:E20)</f>
-        <v>0.16319424672728389</v>
-      </c>
-      <c r="F21" s="27">
-        <f>AVERAGE(F5:F20)</f>
-        <v>2.3856849746975675</v>
-      </c>
-      <c r="G21" s="27">
-        <f>AVERAGE(G5:G20)</f>
-        <v>2.4302891511368241</v>
-      </c>
-      <c r="H21" s="27">
-        <f>AVERAGE(H5:H20)</f>
-        <v>5.1858339990395717</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1907,16 +1931,6 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A5:I20">
@@ -1932,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1944,50 +1958,50 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+    <row r="1" spans="1:17" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="24" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="26" t="s">
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="26"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P2" s="25"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="17" t="s">
         <v>46</v>
@@ -2007,7 +2021,7 @@
       <c r="G3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="30" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="17" t="s">
@@ -2025,17 +2039,17 @@
       <c r="M3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="30" t="s">
         <v>40</v>
       </c>
       <c r="O3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2057,8 +2071,8 @@
       <c r="G4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="21">
-        <v>19.258297634226</v>
+      <c r="H4" s="12">
+        <v>20.079052846840298</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>53</v>
@@ -2070,106 +2084,111 @@
         <v>53</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="21">
-        <v>18.302131042685001</v>
+      <c r="N4" s="12">
+        <v>19.382297485855101</v>
       </c>
       <c r="O4" s="16">
         <v>23</v>
       </c>
-      <c r="P4" s="21">
-        <v>28.0364544246539</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4" s="12">
+        <v>28.9681465159534</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="H5" s="12">
+        <v>27.139027898624001</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="21">
-        <v>25.572059132445698</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="21">
-        <v>4.9908146514642899</v>
+      <c r="N5" s="12">
+        <v>16.541104801067799</v>
       </c>
       <c r="O5" s="16">
-        <v>4</v>
-      </c>
-      <c r="P5" s="21">
-        <v>12.542075440370599</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="P5" s="12">
+        <v>34.577968000324503</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="21">
-        <v>15.253680793260401</v>
+      <c r="G6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="12">
+        <v>30.441160946743601</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N6" s="21">
-        <v>8.05107671260172</v>
+        <v>64</v>
+      </c>
+      <c r="N6" s="12">
+        <v>26.502150372800301</v>
       </c>
       <c r="O6" s="16">
-        <v>3</v>
-      </c>
-      <c r="P6" s="21">
-        <v>14.4859881137053</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="P6" s="12">
+        <v>29.3365801489118</v>
+      </c>
+      <c r="Q6" s="19"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="21">
-        <v>2.6653402118662202</v>
+      <c r="E7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="12">
+        <v>18.116015828497599</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N7" s="21">
-        <v>9.9346644419024592</v>
+      <c r="N7" s="12">
+        <v>25.834055056104699</v>
       </c>
       <c r="O7" s="16">
-        <v>11</v>
-      </c>
-      <c r="P7" s="21">
-        <v>26.8444936387456</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="P7" s="12">
+        <v>44.411756849953001</v>
+      </c>
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>23</v>
       </c>
@@ -2177,387 +2196,380 @@
         <v>56</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="21">
-        <v>18.4687471434437</v>
+        <v>57</v>
+      </c>
+      <c r="H8" s="12">
+        <v>21.165528894888901</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N8" s="21">
-        <v>12.772095375710901</v>
+        <v>63</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N8" s="12">
+        <v>18.666739746079202</v>
       </c>
       <c r="O8" s="16">
-        <v>6</v>
-      </c>
-      <c r="P8" s="21">
-        <v>20.396182601550201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="P8" s="12">
+        <v>24.641402703191901</v>
+      </c>
+      <c r="Q8" s="19"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1.5558533844685001</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" s="12">
+        <v>5.8179929364745702</v>
+      </c>
+      <c r="O9" s="16">
+        <v>3</v>
+      </c>
+      <c r="P9" s="12">
+        <v>11.209225463037001</v>
+      </c>
+      <c r="Q9" s="19"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="21">
-        <v>3.7267889084023</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="12">
+        <v>24.024819490112701</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="12">
+        <v>12.0909139155526</v>
+      </c>
+      <c r="O10" s="16">
+        <v>5</v>
+      </c>
+      <c r="P10" s="12">
+        <v>19.712213531993001</v>
+      </c>
+      <c r="Q10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N9" s="21">
-        <v>1.75350821170257</v>
-      </c>
-      <c r="O9" s="16">
-        <v>4</v>
-      </c>
-      <c r="P9" s="21">
-        <v>11.653545886195401</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="12">
+        <v>27.687600970005601</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="12">
+        <v>10.223110138722401</v>
+      </c>
+      <c r="O11" s="16">
+        <v>6</v>
+      </c>
+      <c r="P11" s="12">
+        <v>30.718900244560999</v>
+      </c>
+      <c r="Q11" s="19"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="12">
+        <v>10.779872100928801</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N12" s="12">
+        <v>9.6749756723765099</v>
+      </c>
+      <c r="O12" s="16">
+        <v>7</v>
+      </c>
+      <c r="P12" s="12">
+        <v>18.702745369786399</v>
+      </c>
+      <c r="Q12" s="19"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="21">
-        <v>5.02761993352616</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="12">
+        <v>54.344361142806797</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="12">
+        <v>29.8773817359647</v>
+      </c>
+      <c r="O13" s="16">
+        <v>21</v>
+      </c>
+      <c r="P13" s="12">
+        <v>61.981173276838902</v>
+      </c>
+      <c r="Q13" s="19"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="21">
-        <v>1.94735924672979</v>
-      </c>
-      <c r="O10" s="16">
-        <v>3</v>
-      </c>
-      <c r="P10" s="21">
-        <v>9.2768475754770492</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="H14" s="12">
+        <v>10.597977336528601</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="21">
-        <v>26.059437976739702</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N11" s="21">
-        <v>9.1920579407900895</v>
-      </c>
-      <c r="O11" s="16">
-        <v>4</v>
-      </c>
-      <c r="P11" s="21">
-        <v>14.082845264175401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="21">
-        <v>11.638227357847301</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N12" s="21">
-        <v>5.0687779206005503</v>
-      </c>
-      <c r="O12" s="16">
-        <v>6</v>
-      </c>
-      <c r="P12" s="21">
-        <v>22.662080848904701</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="21">
-        <v>26.010100533633899</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N13" s="21">
-        <v>14.905735037114599</v>
-      </c>
-      <c r="O13" s="16">
-        <v>6</v>
-      </c>
-      <c r="P13" s="21">
-        <v>29.782942931126598</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="21">
-        <v>21.208504513068</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" s="21">
-        <v>18.227727275701699</v>
+      <c r="N14" s="12">
+        <v>7.2236421328398199</v>
       </c>
       <c r="O14" s="16">
-        <v>14</v>
-      </c>
-      <c r="P14" s="21">
-        <v>31.562227510456498</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="P14" s="12">
+        <v>30.552159858848999</v>
+      </c>
+      <c r="Q14" s="19"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="H15" s="12">
+        <v>23.469860468929198</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="21">
-        <v>15.566052563108199</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N15" s="21">
-        <v>4.8688513242263696</v>
+      <c r="J15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="12">
+        <v>36.401189358596802</v>
       </c>
       <c r="O15" s="16">
-        <v>6</v>
-      </c>
-      <c r="P15" s="21">
-        <v>19.668898911614601</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="P15" s="12">
+        <v>47.869179080141201</v>
+      </c>
+      <c r="Q15" s="19"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="21">
-        <v>16.052952559125799</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>55</v>
+      <c r="H16" s="12">
+        <v>7.5557961539220697</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N16" s="21">
-        <v>20.7374818472559</v>
+        <v>64</v>
+      </c>
+      <c r="N16" s="12">
+        <v>3.84694004446381</v>
       </c>
       <c r="O16" s="16">
         <v>3</v>
       </c>
-      <c r="P16" s="21">
-        <v>21.107540376922</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P16" s="12">
+        <v>9.2393786752182407</v>
+      </c>
+      <c r="Q16" s="19"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H17" s="21">
-        <v>13.8504202936412</v>
-      </c>
-      <c r="M17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N17" s="21">
-        <v>2.1249719994100098</v>
+      <c r="D17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="12">
+        <v>28.3923382760034</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" s="12">
+        <v>17.2954425049831</v>
       </c>
       <c r="O17" s="16">
-        <v>5</v>
-      </c>
-      <c r="P17" s="21">
-        <v>10.938264219051799</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="P17" s="12">
+        <v>35.6423432210416</v>
+      </c>
+      <c r="Q17" s="19"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="21">
-        <v>13.7594512470226</v>
+        <v>57</v>
+      </c>
+      <c r="H18" s="12">
+        <v>14.1358158157293</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="12">
+        <v>15.366018274553101</v>
+      </c>
+      <c r="O18" s="16">
+        <v>6</v>
+      </c>
+      <c r="P18" s="12">
+        <v>24.2443031772175</v>
+      </c>
+      <c r="Q18" s="19"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="12">
+        <v>5.8352171120526304</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N18" s="21">
-        <v>4.9550292596154497</v>
-      </c>
-      <c r="O18" s="16">
-        <v>8</v>
-      </c>
-      <c r="P18" s="21">
-        <v>17.793063649430799</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" s="21">
-        <v>8.2956905296415897</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N19" s="21">
-        <v>2.2124772274328701</v>
+      <c r="N19" s="12">
+        <v>11.6712255204115</v>
       </c>
       <c r="O19" s="16">
         <v>3</v>
       </c>
-      <c r="P19" s="21">
-        <v>8.8535280018722595</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="P19" s="12">
+        <v>13.1553568297421</v>
+      </c>
+      <c r="Q19" s="19"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14">
+        <v>3.83291938858298</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="21">
-        <v>3.54852619634626</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N20" s="21">
-        <v>3.44424651527516</v>
-      </c>
-      <c r="O20" s="16">
-        <v>4</v>
-      </c>
-      <c r="P20" s="21">
-        <v>8.4811994451953403</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="22">
-        <v>17.144184909620201</v>
-      </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="N21" s="22">
-        <v>9.0218271098422296</v>
-      </c>
-      <c r="O21" s="17">
-        <v>6</v>
-      </c>
-      <c r="P21" s="22">
-        <v>25.4568848146839</v>
-      </c>
+      <c r="N20" s="14">
+        <v>13.619076800758901</v>
+      </c>
+      <c r="O20" s="17">
+        <v>5</v>
+      </c>
+      <c r="P20" s="14">
+        <v>18.6154248353239</v>
+      </c>
+      <c r="Q20" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
models should work for POFR and PF, updated figs/tabs
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
   <si>
     <t>Secchi depth (m)</t>
   </si>
@@ -405,6 +405,12 @@
     <t>**-</t>
   </si>
   <si>
+    <t>P. friesii</t>
+  </si>
+  <si>
+    <t>ns+</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -441,7 +447,83 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> and does not consider joint effects with the remaining categories (see Table 2). ***: p ≤ 0.0001, **: p ≤ 0.001, *: p≤ 0.05.</t>
+      <t xml:space="preserve"> and does not consider joint effects with the remaining categories (see Table 2). ***: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; 0.0001, **: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; 0.001, *: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; 0.05, ns: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ≥ 0.05.</t>
     </r>
   </si>
 </sst>
@@ -512,7 +594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -540,20 +622,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -586,9 +659,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -597,7 +667,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -610,18 +682,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,13 +976,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1175,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1196,570 +1256,565 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="12">
         <v>3.8259046021258598</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="12">
         <v>0.63218151361807995</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="12">
         <v>6.6330984986780397</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="12">
         <v>0.33220179258222099</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="12">
         <v>6.1657584622845398</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="12">
         <v>3.38036039408495</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="12">
         <v>11.844547267379699</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="12">
         <v>32.814052530753401</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="29">
-        <v>11.528157280018499</v>
-      </c>
-      <c r="C4" s="29">
-        <v>-0.39906133671750998</v>
-      </c>
-      <c r="D4" s="29">
-        <v>13.7694529306793</v>
-      </c>
-      <c r="E4" s="29">
-        <v>0.108096301396055</v>
-      </c>
-      <c r="F4" s="29">
-        <v>5.3057407524357396</v>
-      </c>
-      <c r="G4" s="29">
-        <v>3.9764452332559399</v>
-      </c>
-      <c r="H4" s="29">
-        <v>11.526329083953501</v>
-      </c>
-      <c r="I4" s="29">
-        <v>45.815160245021602</v>
+      <c r="B4" s="12">
+        <v>11.6629156353062</v>
+      </c>
+      <c r="C4" s="12">
+        <v>-0.468546048098684</v>
+      </c>
+      <c r="D4" s="12">
+        <v>14.9441773979804</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.31048354749038098</v>
+      </c>
+      <c r="F4" s="12">
+        <v>5.3752254638169097</v>
+      </c>
+      <c r="G4" s="12">
+        <v>3.8416868779682498</v>
+      </c>
+      <c r="H4" s="12">
+        <v>11.3239418378592</v>
+      </c>
+      <c r="I4" s="12">
+        <v>46.989884712322599</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="29">
-        <v>3.67524595560204</v>
-      </c>
-      <c r="C5" s="29">
-        <v>0.63619684933756704</v>
-      </c>
-      <c r="D5" s="29">
-        <v>3.2920969463023102</v>
-      </c>
-      <c r="E5" s="29">
-        <v>2.7172877415922301</v>
-      </c>
-      <c r="F5" s="29">
-        <v>1.99585595306025</v>
-      </c>
-      <c r="G5" s="29">
-        <v>2.8958174207390202</v>
-      </c>
-      <c r="H5" s="29">
-        <v>21.152809828810199</v>
-      </c>
-      <c r="I5" s="29">
-        <v>36.365310695443597</v>
+      <c r="B5" s="12">
+        <v>3.8256224295928498</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1.4290003808057701</v>
+      </c>
+      <c r="D5" s="12">
+        <v>3.1529726264681299</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2.8053955750982902</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1.2030524215920499</v>
+      </c>
+      <c r="G5" s="12">
+        <v>2.7454409467482099</v>
+      </c>
+      <c r="H5" s="12">
+        <v>21.064701995304201</v>
+      </c>
+      <c r="I5" s="12">
+        <v>36.226186375609501</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="12">
         <v>2.3372047737642601</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="12">
         <v>-8.7018648078196495E-2</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="12">
         <v>20.016525895666199</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="12">
         <v>0.68552936784267404</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="12">
         <v>9.3019492673961608</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="12">
         <v>-0.84031338205338102</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="12">
         <v>15.933595068944101</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="12">
         <v>47.347472343481797</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="29">
-        <v>0.98940903130942903</v>
-      </c>
-      <c r="C7" s="29">
-        <v>2.2247251257090799</v>
-      </c>
-      <c r="D7" s="29">
-        <v>3.0884995219489801</v>
-      </c>
-      <c r="E7" s="29">
-        <v>0.36944645829869399</v>
-      </c>
-      <c r="F7" s="29">
-        <v>1.74622977596202</v>
-      </c>
-      <c r="G7" s="29">
-        <v>5.4803350191714602</v>
-      </c>
-      <c r="H7" s="29">
-        <v>14.326338386109301</v>
-      </c>
-      <c r="I7" s="29">
-        <v>28.224983318509</v>
+      <c r="B7" s="12">
+        <v>1.4140390948910799</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2.4797405741260001</v>
+      </c>
+      <c r="D7" s="12">
+        <v>3.0430025716074298</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.78956039054747196</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1.4912143275451</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5.0557049555897997</v>
+      </c>
+      <c r="H7" s="12">
+        <v>13.906224453860601</v>
+      </c>
+      <c r="I7" s="12">
+        <v>28.179486368167399</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="12">
         <v>7.7116585255798703E-2</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="12">
         <v>2.0930214857060299</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="12">
         <v>7.6929038157176102</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="12">
         <v>-0.28718401809252297</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="12">
         <v>1.75040083001413</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="12">
         <v>-0.49583382154171401</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="12">
         <v>2.2617546388469401</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="12">
         <v>13.092179515906301</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.98357968718654198</v>
+      </c>
+      <c r="C9" s="12">
+        <v>-0.16049003662514899</v>
+      </c>
+      <c r="D9" s="12">
+        <v>9.2210975281220193</v>
+      </c>
+      <c r="E9" s="12">
+        <v>2.9699712932107498E-2</v>
+      </c>
+      <c r="F9" s="12">
+        <v>5.8704436149719097</v>
+      </c>
+      <c r="G9" s="12">
+        <v>-1.16381778006093</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1.4845048442500799</v>
+      </c>
+      <c r="I9" s="12">
+        <v>16.2650175707766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B10" s="12">
         <v>13.981264010342599</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C10" s="12">
         <v>0.35003000383149202</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D10" s="12">
         <v>7.5918874075822096</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E10" s="12">
         <v>1.86981289264796</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F10" s="12">
         <v>3.9465835372886602</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G10" s="12">
         <v>2.2492551053376899</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H10" s="12">
         <v>5.9244874817844702</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I10" s="12">
         <v>35.913320438814999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="29">
-        <v>12.022892934780399</v>
-      </c>
-      <c r="C10" s="29">
-        <v>0.85018854770078101</v>
-      </c>
-      <c r="D10" s="29">
-        <v>10.2667558804467</v>
-      </c>
-      <c r="E10" s="29">
-        <v>-0.78072047573788395</v>
-      </c>
-      <c r="F10" s="29">
-        <v>4.0067158531511398</v>
-      </c>
-      <c r="G10" s="29">
-        <v>10.2985022973547</v>
-      </c>
-      <c r="H10" s="29">
-        <v>6.1469262136083698</v>
-      </c>
-      <c r="I10" s="29">
-        <v>42.811261251304202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="B11" s="12">
+        <v>11.4524142302475</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.55776277767140003</v>
+      </c>
+      <c r="D11" s="12">
+        <v>10.3352750862135</v>
+      </c>
+      <c r="E11" s="12">
+        <v>-0.83670047005383097</v>
+      </c>
+      <c r="F11" s="12">
+        <v>4.2991416231805202</v>
+      </c>
+      <c r="G11" s="12">
+        <v>10.868981001887599</v>
+      </c>
+      <c r="H11" s="12">
+        <v>6.20290620792432</v>
+      </c>
+      <c r="I11" s="12">
+        <v>42.879780457071</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B12" s="12">
         <v>4.0312116339573798</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C12" s="12">
         <v>-0.32605531797234</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D12" s="12">
         <v>7.2822142948131701</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E12" s="12">
         <v>-3.7973580591921199E-2</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F12" s="12">
         <v>4.6338970274099198</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G12" s="12">
         <v>1.38152650403249</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H12" s="12">
         <v>5.4051075435308498</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I12" s="12">
         <v>22.3699281051795</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B13" s="12">
         <v>5.86416232548794</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C13" s="12">
         <v>-0.15893741171891801</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D13" s="12">
         <v>13.0006647662969</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E13" s="12">
         <v>0.16932059242872299</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F13" s="12">
         <v>0.66963028565191196</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G13" s="12">
         <v>19.1135099552871</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H13" s="12">
         <v>29.1973682696031</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I13" s="12">
         <v>67.855718783036707</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="29">
-        <v>1.8516155304474899</v>
-      </c>
-      <c r="C13" s="29">
-        <v>-0.30751293607740299</v>
-      </c>
-      <c r="D13" s="29">
-        <v>17.146871713932899</v>
-      </c>
-      <c r="E13" s="29">
-        <v>-1.0499248374495901E-2</v>
-      </c>
-      <c r="F13" s="29">
-        <v>4.6484270904603902</v>
-      </c>
-      <c r="G13" s="29">
-        <v>5.8636338276242803</v>
-      </c>
-      <c r="H13" s="29">
-        <v>2.8932272268313199</v>
-      </c>
-      <c r="I13" s="29">
-        <v>32.085763204844497</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="B14" s="12">
+        <v>1.8958099806787401</v>
+      </c>
+      <c r="C14" s="12">
+        <v>-0.34030989754139102</v>
+      </c>
+      <c r="D14" s="12">
+        <v>16.1064209908237</v>
+      </c>
+      <c r="E14" s="12">
+        <v>-6.9880611125117103E-3</v>
+      </c>
+      <c r="F14" s="12">
+        <v>4.6812240519243797</v>
+      </c>
+      <c r="G14" s="12">
+        <v>5.8194393773930297</v>
+      </c>
+      <c r="H14" s="12">
+        <v>2.88971603956933</v>
+      </c>
+      <c r="I14" s="12">
+        <v>31.045312481735301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="29">
-        <v>-3.7712740313389198E-2</v>
-      </c>
-      <c r="C14" s="29">
-        <v>0.97570126684389802</v>
-      </c>
-      <c r="D14" s="29">
-        <v>8.1552200772493997</v>
-      </c>
-      <c r="E14" s="29">
-        <v>8.50590770211435E-2</v>
-      </c>
-      <c r="F14" s="29">
-        <v>15.5469863625242</v>
-      </c>
-      <c r="G14" s="29">
-        <v>3.6290714800138799</v>
-      </c>
-      <c r="H14" s="29">
-        <v>19.793442652207599</v>
-      </c>
-      <c r="I14" s="29">
-        <v>48.147768175546702</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="B15" s="12">
+        <v>-0.17397088949846501</v>
+      </c>
+      <c r="C15" s="12">
+        <v>2.7767948765934198</v>
+      </c>
+      <c r="D15" s="12">
+        <v>8.6129188796417004</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0.18322529873927601</v>
+      </c>
+      <c r="F15" s="12">
+        <v>15.7956541408111</v>
+      </c>
+      <c r="G15" s="12">
+        <v>3.5403792095692199</v>
+      </c>
+      <c r="H15" s="12">
+        <v>19.920226850119199</v>
+      </c>
+      <c r="I15" s="12">
+        <v>50.655228365975503</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="29">
-        <v>4.6418657411277504</v>
-      </c>
-      <c r="C15" s="29">
-        <v>0.45480373995631102</v>
-      </c>
-      <c r="D15" s="29">
-        <v>5.7999705323769204</v>
-      </c>
-      <c r="E15" s="29">
-        <v>0.58691838065637603</v>
-      </c>
-      <c r="F15" s="29">
-        <v>1.11239611070338</v>
-      </c>
-      <c r="G15" s="29">
-        <v>0.63419021899022698</v>
-      </c>
-      <c r="H15" s="29">
-        <v>1.69282181314772</v>
-      </c>
-      <c r="I15" s="29">
-        <v>14.9229665369587</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="B16" s="12">
+        <v>4.6066897736289603</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1.0381192244474999</v>
+      </c>
+      <c r="D16" s="12">
+        <v>6.1915490826149604</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1.7715636864132001</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0.52908062621219698</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.66936618648901802</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.50817650739088904</v>
+      </c>
+      <c r="I16" s="12">
+        <v>15.3145450871967</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="29">
-        <v>8.2489420956514206</v>
-      </c>
-      <c r="C16" s="29">
-        <v>0.10002970178533099</v>
-      </c>
-      <c r="D16" s="29">
-        <v>12.0963518683893</v>
-      </c>
-      <c r="E16" s="29">
-        <v>-0.41700196504258502</v>
-      </c>
-      <c r="F16" s="29">
-        <v>0.99205307178151803</v>
-      </c>
-      <c r="G16" s="29">
-        <v>3.94003644893575</v>
-      </c>
-      <c r="H16" s="29">
-        <v>16.620361696458801</v>
-      </c>
-      <c r="I16" s="29">
-        <v>41.5807729179596</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="B17" s="12">
+        <v>7.5536840274200898</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.38342219619218498</v>
+      </c>
+      <c r="D17" s="12">
+        <v>13.5389172339701</v>
+      </c>
+      <c r="E17" s="12">
+        <v>-0.55611116111349301</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.70866057737466503</v>
+      </c>
+      <c r="G17" s="12">
+        <v>4.6352945171670799</v>
+      </c>
+      <c r="H17" s="12">
+        <v>16.759470892529698</v>
+      </c>
+      <c r="I17" s="12">
+        <v>43.023338283540298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="29">
-        <v>2.0372848390243399</v>
-      </c>
-      <c r="C17" s="29">
-        <v>0.286527114234159</v>
-      </c>
-      <c r="D17" s="29">
-        <v>7.3159369089321498</v>
-      </c>
-      <c r="E17" s="29">
-        <v>0.28891363718901403</v>
-      </c>
-      <c r="F17" s="29">
-        <v>6.1746497224714796</v>
-      </c>
-      <c r="G17" s="29">
-        <v>3.19368953885746</v>
-      </c>
-      <c r="H17" s="29">
-        <v>8.6159278006584508</v>
-      </c>
-      <c r="I17" s="29">
-        <v>27.9129295613671</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="B18" s="12">
+        <v>2.2801732314539298</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.24120969460436101</v>
+      </c>
+      <c r="D18" s="12">
+        <v>6.3921056697163099</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0.22341221887547399</v>
+      </c>
+      <c r="F18" s="12">
+        <v>6.2199671421012797</v>
+      </c>
+      <c r="G18" s="12">
+        <v>2.9508011464278701</v>
+      </c>
+      <c r="H18" s="12">
+        <v>8.6814292189719904</v>
+      </c>
+      <c r="I18" s="12">
+        <v>26.9890983221512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B19" s="12">
         <v>-0.29360900539779899</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C19" s="12">
         <v>0.72891679040278901</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D19" s="12">
         <v>0.41902386699275201</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E19" s="12">
         <v>0.122246570823836</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F19" s="12">
         <v>5.1835460768454498</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G19" s="12">
         <v>0.37006346428718501</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H19" s="12">
         <v>5.6365160823393996</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I19" s="12">
         <v>12.166703846293601</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="14">
-        <v>0.14655107668312101</v>
-      </c>
-      <c r="C19" s="14">
-        <v>0.43201004064258303</v>
-      </c>
-      <c r="D19" s="14">
-        <v>5.3823753575645004</v>
-      </c>
-      <c r="E19" s="14">
-        <v>0.42279392187943898</v>
-      </c>
-      <c r="F19" s="14">
-        <v>9.9694750877389993</v>
-      </c>
-      <c r="G19" s="14">
-        <v>0.46877663952258303</v>
-      </c>
-      <c r="H19" s="14">
-        <v>2.7947977504978301</v>
-      </c>
-      <c r="I19" s="14">
-        <v>19.616779874529101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="21">
-        <f>AVERAGE(B5:B19)</f>
-        <v>3.9715629858481858</v>
-      </c>
-      <c r="C20" s="21">
-        <f t="shared" ref="C20:I20" si="0">AVERAGE(C5:C19)</f>
-        <v>0.55017509015354427</v>
-      </c>
-      <c r="D20" s="21">
-        <f t="shared" si="0"/>
-        <v>8.5698199236141317</v>
-      </c>
-      <c r="E20" s="21">
-        <f t="shared" si="0"/>
-        <v>0.38559662350271195</v>
-      </c>
-      <c r="F20" s="21">
-        <f t="shared" si="0"/>
-        <v>4.7785864034973065</v>
-      </c>
-      <c r="G20" s="21">
-        <f t="shared" si="0"/>
-        <v>3.8788173811039157</v>
-      </c>
-      <c r="H20" s="21">
-        <f t="shared" si="0"/>
-        <v>10.559698830225228</v>
-      </c>
-      <c r="I20" s="21">
-        <f t="shared" si="0"/>
-        <v>32.694257237945031</v>
+      <c r="B20" s="14">
+        <v>0.279275362119003</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0.38778534662922098</v>
+      </c>
+      <c r="D20" s="14">
+        <v>4.2799749206066799</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.45301890089656199</v>
+      </c>
+      <c r="F20" s="14">
+        <v>10.0136997817524</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0.33605235408670198</v>
+      </c>
+      <c r="H20" s="14">
+        <v>2.7645727714807098</v>
+      </c>
+      <c r="I20" s="14">
+        <v>18.514379437571201</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1901,36 +1956,6 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A5:I20">
@@ -1946,10 +1971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1959,93 +1984,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="A1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="23" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="25" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="25"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2092,11 +2117,11 @@
       <c r="N4" s="12">
         <v>19.382297485855101</v>
       </c>
-      <c r="O4" s="16">
-        <v>23</v>
+      <c r="O4" s="11">
+        <v>22</v>
       </c>
       <c r="P4" s="12">
-        <v>28.9681465159534</v>
+        <v>28.705577979771601</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2121,15 +2146,15 @@
       <c r="N5" s="12">
         <v>16.541104801067799</v>
       </c>
-      <c r="O5" s="16">
-        <v>10</v>
+      <c r="O5" s="11">
+        <v>12</v>
       </c>
       <c r="P5" s="12">
-        <v>34.577968000324503</v>
+        <v>36.3477779938219</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2144,22 +2169,25 @@
       <c r="J6" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="L6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="N6" s="12">
         <v>26.502150372800301</v>
       </c>
-      <c r="O6" s="16">
+      <c r="O6" s="11">
         <v>8</v>
       </c>
       <c r="P6" s="12">
         <v>29.3365801489118</v>
       </c>
-      <c r="Q6" s="19"/>
+      <c r="Q6" s="18"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2180,16 +2208,16 @@
       <c r="N7" s="12">
         <v>25.834055056104699</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="11">
         <v>12</v>
       </c>
       <c r="P7" s="12">
         <v>44.411756849953001</v>
       </c>
-      <c r="Q7" s="19"/>
+      <c r="Q7" s="18"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2213,16 +2241,16 @@
       <c r="N8" s="12">
         <v>18.666739746079202</v>
       </c>
-      <c r="O8" s="16">
-        <v>8</v>
+      <c r="O8" s="11">
+        <v>6</v>
       </c>
       <c r="P8" s="12">
-        <v>24.641402703191901</v>
-      </c>
-      <c r="Q8" s="19"/>
+        <v>22.324660404927201</v>
+      </c>
+      <c r="Q8" s="18"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2237,339 +2265,362 @@
       <c r="N9" s="12">
         <v>5.8179929364745702</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="11">
         <v>3</v>
       </c>
       <c r="P9" s="12">
         <v>11.209225463037001</v>
       </c>
-      <c r="Q9" s="19"/>
+      <c r="Q9" s="18"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1.3339664643078</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="12">
+        <v>7.2241581355289499</v>
+      </c>
+      <c r="O10" s="11">
+        <v>11</v>
+      </c>
+      <c r="P10" s="12">
+        <v>20.3188255378567</v>
+      </c>
+      <c r="Q10" s="18"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>24</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="12">
-        <v>24.024819490112701</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N10" s="12">
-        <v>12.0909139155526</v>
-      </c>
-      <c r="O10" s="16">
-        <v>5</v>
-      </c>
-      <c r="P10" s="12">
-        <v>19.712213531993001</v>
-      </c>
-      <c r="Q10" s="19"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="12">
+        <v>24.024819490112701</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="12">
-        <v>27.687600970005601</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="N11" s="12">
+        <v>12.0909139155526</v>
+      </c>
+      <c r="O11" s="11">
+        <v>5</v>
+      </c>
+      <c r="P11" s="12">
+        <v>19.712213531993001</v>
+      </c>
+      <c r="Q11" s="18"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="N11" s="12">
-        <v>10.223110138722401</v>
-      </c>
-      <c r="O11" s="16">
-        <v>6</v>
-      </c>
-      <c r="P11" s="12">
-        <v>30.718900244560999</v>
-      </c>
-      <c r="Q11" s="19"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="12">
+        <v>27.687600970005601</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="12">
+      <c r="N12" s="12">
+        <v>10.223110138722401</v>
+      </c>
+      <c r="O12" s="11">
+        <v>6</v>
+      </c>
+      <c r="P12" s="12">
+        <v>30.718900244560999</v>
+      </c>
+      <c r="Q12" s="18"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="12">
         <v>10.779872100928801</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N13" s="12">
         <v>9.6749756723765099</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O13" s="11">
         <v>7</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P13" s="12">
         <v>18.702745369786399</v>
       </c>
-      <c r="Q12" s="19"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="Q13" s="18"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H14" s="12">
         <v>54.344361142806797</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N14" s="12">
         <v>29.8773817359647</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O14" s="11">
         <v>21</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P14" s="12">
         <v>61.981173276838902</v>
       </c>
-      <c r="Q13" s="19"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H15" s="12">
         <v>10.597977336528601</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N15" s="12">
         <v>7.2236421328398199</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O15" s="11">
         <v>10</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P15" s="12">
         <v>30.552159858848999</v>
       </c>
-      <c r="Q14" s="19"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="Q15" s="18"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H16" s="12">
         <v>23.469860468929198</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N15" s="12">
+      <c r="N16" s="12">
         <v>36.401189358596802</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O16" s="11">
         <v>8</v>
       </c>
-      <c r="P15" s="12">
+      <c r="P16" s="12">
         <v>47.869179080141201</v>
       </c>
-      <c r="Q15" s="19"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="Q16" s="18"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H17" s="12">
         <v>7.5557961539220697</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N17" s="12">
         <v>3.84694004446381</v>
       </c>
-      <c r="O16" s="16">
-        <v>3</v>
-      </c>
-      <c r="P16" s="12">
-        <v>9.2393786752182407</v>
-      </c>
-      <c r="Q16" s="19"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="O17" s="11">
+        <v>4</v>
+      </c>
+      <c r="P17" s="12">
+        <v>10.2968701347048</v>
+      </c>
+      <c r="Q17" s="18"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="12">
-        <v>28.3923382760034</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N17" s="12">
-        <v>17.2954425049831</v>
-      </c>
-      <c r="O17" s="16">
-        <v>11</v>
-      </c>
-      <c r="P17" s="12">
-        <v>35.6423432210416</v>
-      </c>
-      <c r="Q17" s="19"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H18" s="12">
+        <v>28.3923382760034</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" s="12">
+        <v>17.2954425049831</v>
+      </c>
+      <c r="O18" s="11">
+        <v>11</v>
+      </c>
+      <c r="P18" s="12">
+        <v>35.6423432210416</v>
+      </c>
+      <c r="Q18" s="18"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="12">
         <v>14.1358158157293</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N19" s="12">
         <v>15.366018274553101</v>
       </c>
-      <c r="O18" s="16">
-        <v>6</v>
-      </c>
-      <c r="P18" s="12">
-        <v>24.2443031772175</v>
-      </c>
-      <c r="Q18" s="19"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="O19" s="11">
+        <v>5</v>
+      </c>
+      <c r="P19" s="12">
+        <v>22.996617986328001</v>
+      </c>
+      <c r="Q19" s="18"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H20" s="12">
         <v>5.8352171120526304</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N20" s="12">
         <v>11.6712255204115</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O20" s="11">
         <v>3</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P20" s="12">
         <v>13.1553568297421</v>
       </c>
-      <c r="Q19" s="19"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="Q20" s="18"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14">
         <v>3.83291938858298</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13" t="s">
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N21" s="14">
         <v>13.619076800758901</v>
       </c>
-      <c r="O20" s="17">
+      <c r="O21" s="20">
         <v>5</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P21" s="14">
         <v>18.6154248353239</v>
       </c>
-      <c r="Q20" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
text updated for freq occurrence
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -626,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -682,6 +682,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1238,7 +1239,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1818,14 +1819,38 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="B21" s="25">
+        <f>AVERAGE(B5:B20)</f>
+        <v>3.7571667031956508</v>
+      </c>
+      <c r="C21" s="25">
+        <f t="shared" ref="C21:I21" si="0">AVERAGE(C5:C20)</f>
+        <v>0.7120620024421358</v>
+      </c>
+      <c r="D21" s="25">
+        <f t="shared" si="0"/>
+        <v>8.5548409148033357</v>
+      </c>
+      <c r="E21" s="25">
+        <f t="shared" si="0"/>
+        <v>0.46111424476758095</v>
+      </c>
+      <c r="F21" s="25">
+        <f t="shared" si="0"/>
+        <v>4.76863408325449</v>
+      </c>
+      <c r="G21" s="25">
+        <f t="shared" si="0"/>
+        <v>3.5772406087904352</v>
+      </c>
+      <c r="H21" s="25">
+        <f t="shared" si="0"/>
+        <v>9.9087974291531182</v>
+      </c>
+      <c r="I21" s="25">
+        <f t="shared" si="0"/>
+        <v>31.739855986406727</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
@@ -1974,7 +1999,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new table of spp eco added
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="10275"/>
   </bookViews>
   <sheets>
-    <sheet name="Table1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table1" sheetId="4" r:id="rId1"/>
+    <sheet name="Table2" sheetId="1" r:id="rId2"/>
+    <sheet name="Table3" sheetId="2" r:id="rId3"/>
+    <sheet name="Table4" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="120">
   <si>
     <t>Secchi depth (m)</t>
   </si>
@@ -111,6 +112,223 @@
     <t>Local variables</t>
   </si>
   <si>
+    <t>Climate variables</t>
+  </si>
+  <si>
+    <r>
+      <t>Alkalinity (mg L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> CaCO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Color (Pt-Co units)</t>
+  </si>
+  <si>
+    <r>
+      <t>Total phosphorus (mg L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Richness</t>
+  </si>
+  <si>
+    <t>Assemb. comp.</t>
+  </si>
+  <si>
+    <t>P. amplifolius</t>
+  </si>
+  <si>
+    <t>P. crispus</t>
+  </si>
+  <si>
+    <t>P. epihydrus</t>
+  </si>
+  <si>
+    <t>P. gramineus</t>
+  </si>
+  <si>
+    <t>P. illinoensis</t>
+  </si>
+  <si>
+    <t>P. natans</t>
+  </si>
+  <si>
+    <t>P. pectinatus</t>
+  </si>
+  <si>
+    <t>P. praelongus</t>
+  </si>
+  <si>
+    <t>P. pusillus</t>
+  </si>
+  <si>
+    <t>P. robbinsii</t>
+  </si>
+  <si>
+    <t>P. zosteriformis</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Local + Climate</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Climate + Space</t>
+  </si>
+  <si>
+    <t>Local + Space</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>P. richardsoni</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>prec</t>
+  </si>
+  <si>
+    <t>tmax</t>
+  </si>
+  <si>
+    <t>tmean</t>
+  </si>
+  <si>
+    <t>tmin</t>
+  </si>
+  <si>
+    <t>alk</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>secchi</t>
+  </si>
+  <si>
+    <t>tp</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>***+</t>
+  </si>
+  <si>
+    <t>***-</t>
+  </si>
+  <si>
+    <t>*+</t>
+  </si>
+  <si>
+    <t>P. foliosus</t>
+  </si>
+  <si>
+    <t>P. spirillus</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>P. strictifolius</t>
+  </si>
+  <si>
+    <t>**+</t>
+  </si>
+  <si>
+    <t>*-</t>
+  </si>
+  <si>
+    <t>**-</t>
+  </si>
+  <si>
+    <t>P. friesii</t>
+  </si>
+  <si>
+    <t>ns+</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -119,7 +337,175 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Table 1 </t>
+      <t>Table 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Significant explanatory variables (i.e. local, climate and space variables) demonstrated by selection techniques.  Values are from individual models by category as input to variation partitioning analyses.  Direction of the effect is indicated by + and – symbols from the selected regression model, excluding results for assemblage composition that modelled mutiple species with redundancy analysis.  Empty space means that the variable was not selected for the response. For spatial variables, only the number of selected significant eigenvectors is shown. Explained variance (%) indicates how much the model explains the dependent variable based on adjusted R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and does not consider joint effects with the remaining categories (see Table 2). ***: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; 0.0001, **: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; 0.001, *: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; 0.05, ns: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ≥ 0.05.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Explained variance of assemblage composition, total species richness, and individual </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>Potamogeton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> species among local, climate, and space variables.  Values are adjusted R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Peres-Neto et al. 2006) from partial redundancy analysis and partial least squares.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Table 2 </t>
     </r>
     <r>
       <rPr>
@@ -142,21 +528,165 @@
     </r>
   </si>
   <si>
-    <t>Climate variables</t>
-  </si>
-  <si>
-    <r>
-      <t>Alkalinity (mg L</t>
-    </r>
+    <t>NCHF (78)</t>
+  </si>
+  <si>
+    <t>NGP (3)</t>
+  </si>
+  <si>
+    <t>mean (min - max)</t>
+  </si>
+  <si>
+    <t>WCBP (11)</t>
+  </si>
+  <si>
+    <t>NLF (122)</t>
+  </si>
+  <si>
+    <t>0.12 (0-0.57)</t>
+  </si>
+  <si>
+    <t>0 (0-0)</t>
+  </si>
+  <si>
+    <t>0.29 (0-0.78)</t>
+  </si>
+  <si>
+    <t>0.01 (0-0.15)</t>
+  </si>
+  <si>
+    <t>0.31 (0-0.93)</t>
+  </si>
+  <si>
+    <t>0.08 (0-0.67)</t>
+  </si>
+  <si>
+    <t>0.41 (0-0.86)</t>
+  </si>
+  <si>
+    <t>0.01 (0-0.34)</t>
+  </si>
+  <si>
+    <t>0.07 (0-0.64)</t>
+  </si>
+  <si>
+    <t>0.01 (0-0.41)</t>
+  </si>
+  <si>
+    <t>0.14 (0-0.42)</t>
+  </si>
+  <si>
+    <t>0.04 (0-0.48)</t>
+  </si>
+  <si>
+    <t>0.09 (0-0.64)</t>
+  </si>
+  <si>
+    <t>0.2 (0-0.59)</t>
+  </si>
+  <si>
+    <t>0.1 (0-0.6)</t>
+  </si>
+  <si>
+    <t>0.1 (0-0.45)</t>
+  </si>
+  <si>
+    <t>0.08 (0-0.64)</t>
+  </si>
+  <si>
+    <t>0.18 (0-0.55)</t>
+  </si>
+  <si>
+    <t>0.16 (0-0.71)</t>
+  </si>
+  <si>
+    <t>0.14 (0-0.69)</t>
+  </si>
+  <si>
+    <t>0.03 (0-0.32)</t>
+  </si>
+  <si>
+    <t>0.08 (0-0.4)</t>
+  </si>
+  <si>
+    <t>0.14 (0-0.68)</t>
+  </si>
+  <si>
+    <t>0.02 (0-0.25)</t>
+  </si>
+  <si>
+    <t>0.35 (0-0.84)</t>
+  </si>
+  <si>
+    <t>0.42 (0-0.64)</t>
+  </si>
+  <si>
+    <t>0.11 (0-0.4)</t>
+  </si>
+  <si>
+    <t>0.6 (0.34-1)</t>
+  </si>
+  <si>
+    <t>0.21 (0-0.7)</t>
+  </si>
+  <si>
+    <t>0.08 (0-0.66)</t>
+  </si>
+  <si>
+    <t>0.17 (0-0.92)</t>
+  </si>
+  <si>
+    <t>0.18 (0-0.51)</t>
+  </si>
+  <si>
+    <t>0.37 (0-0.61)</t>
+  </si>
+  <si>
+    <t>0.21 (0-0.56)</t>
+  </si>
+  <si>
+    <t>0.18 (0-0.64)</t>
+  </si>
+  <si>
+    <t>0.08 (0-0.69)</t>
+  </si>
+  <si>
+    <t>0.2 (0-1)</t>
+  </si>
+  <si>
+    <t>0 (0-0.27)</t>
+  </si>
+  <si>
+    <t>0.04 (0-0.62)</t>
+  </si>
+  <si>
+    <t>0.02 (0-0.51)</t>
+  </si>
+  <si>
+    <t>0.06 (0-0.85)</t>
+  </si>
+  <si>
+    <t>0.29 (0-0.75)</t>
+  </si>
+  <si>
+    <t>0.07 (0-0.21)</t>
+  </si>
+  <si>
+    <t>0.34 (0-0.94)</t>
+  </si>
+  <si>
+    <t>0.21 (0-0.61)</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <vertAlign val="superscript"/>
+        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t>-1</t>
+      <t>Table 1</t>
     </r>
     <r>
       <rPr>
@@ -165,196 +695,7 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> CaCO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Color (Pt-Co units)</t>
-  </si>
-  <si>
-    <r>
-      <t>Total phosphorus (mg L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Richness</t>
-  </si>
-  <si>
-    <t>Assemb. comp.</t>
-  </si>
-  <si>
-    <t>P. amplifolius</t>
-  </si>
-  <si>
-    <t>P. crispus</t>
-  </si>
-  <si>
-    <t>P. epihydrus</t>
-  </si>
-  <si>
-    <t>P. gramineus</t>
-  </si>
-  <si>
-    <t>P. illinoensis</t>
-  </si>
-  <si>
-    <t>P. natans</t>
-  </si>
-  <si>
-    <t>P. pectinatus</t>
-  </si>
-  <si>
-    <t>P. praelongus</t>
-  </si>
-  <si>
-    <t>P. pusillus</t>
-  </si>
-  <si>
-    <t>P. robbinsii</t>
-  </si>
-  <si>
-    <t>P. zosteriformis</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Local + Climate</t>
-  </si>
-  <si>
-    <t>Climate</t>
-  </si>
-  <si>
-    <t>Climate + Space</t>
-  </si>
-  <si>
-    <t>Local + Space</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>Space</t>
-  </si>
-  <si>
-    <t>P. richardsoni</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>alt</t>
-  </si>
-  <si>
-    <t>prec</t>
-  </si>
-  <si>
-    <t>tmax</t>
-  </si>
-  <si>
-    <t>tmean</t>
-  </si>
-  <si>
-    <t>tmin</t>
-  </si>
-  <si>
-    <t>alk</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>depth</t>
-  </si>
-  <si>
-    <t>secchi</t>
-  </si>
-  <si>
-    <t>tp</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>***+</t>
-  </si>
-  <si>
-    <t>***-</t>
-  </si>
-  <si>
-    <t>*+</t>
-  </si>
-  <si>
-    <t>P. foliosus</t>
-  </si>
-  <si>
-    <t>P. spirillus</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>P. strictifolius</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Table 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Explained variance of assemblage composition, total species richness, and individual </t>
+      <t xml:space="preserve"> Summary of </t>
     </r>
     <r>
       <rPr>
@@ -373,157 +714,7 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> species among local, climate, and space variables.  Values are adjusted R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (Peres-Neto et al. 2006) from partial redundancy analysis and partial least squares.</t>
-    </r>
-  </si>
-  <si>
-    <t>**+</t>
-  </si>
-  <si>
-    <t>*-</t>
-  </si>
-  <si>
-    <t>**-</t>
-  </si>
-  <si>
-    <t>P. friesii</t>
-  </si>
-  <si>
-    <t>ns+</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>Table 3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Significant explanatory variables (i.e. local, climate and space variables) demonstrated by selection techniques.  Values are from individual models by category as input to variation partitioning analyses.  Direction of the effect is indicated by + and – symbols from the selected regression model, excluding results for assemblage composition that modelled mutiple species with redundancy analysis.  Empty space means that the variable was not selected for the response. For spatial variables, only the number of selected significant eigenvectors is shown. Explained variance (%) indicates how much the model explains the dependent variable based on adjusted R</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> and does not consider joint effects with the remaining categories (see Table 2). ***: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt; 0.0001, **: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt; 0.001, *: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt; 0.05, ns: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> ≥ 0.05.</t>
+      <t xml:space="preserve"> distribution by ecoregion (level III, Omernik 1987).  Species shown are those with variation partitioning models in Figure 3. The mean, minimum, and maximum are based on frequency occurrence values by lake.  Lake counts in each ecoregion are in parentheses by the labels. NCHF: Northern Lakes and Forests Ecoregion, NGP: Northern Glaciated Plains, NLF: Northern Lakes and Forests, WCBP: Western Cornbelt Plains.</t>
     </r>
   </si>
 </sst>
@@ -626,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -670,6 +861,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -682,7 +874,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,10 +1160,567 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27">
+        <v>29</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="27">
+        <v>100</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="27">
+        <v>1</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="27">
+        <v>50</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="27">
+        <v>26</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="27">
+        <v>8</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27">
+        <v>2</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="27">
+        <v>27</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="27">
+        <v>3</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="27">
+        <v>1</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="27">
+        <v>17</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="27">
+        <v>22</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="27">
+        <v>41</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="27">
+        <v>3</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="27">
+        <v>19</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="27">
+        <v>72</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="27">
+        <v>36</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="27">
+        <v>0</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="27">
+        <v>54</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="27">
+        <v>1</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="27">
+        <v>24</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="27">
+        <v>0</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="27">
+        <v>61</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="27">
+        <v>1</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="27">
+        <v>66</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="27">
+        <v>2</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="27">
+        <v>50</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="27">
+        <v>11</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="27">
+        <v>37</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="27">
+        <v>0</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="27">
+        <v>80</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="27">
+        <v>1</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="27">
+        <v>16</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="27">
+        <v>0</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="27">
+        <v>48</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="27">
+        <v>0</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="27">
+        <v>40</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="27">
+        <v>2</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="27">
+        <v>82</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="27">
+        <v>4</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="27">
+        <v>15</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="27">
+        <v>0</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="27">
+        <v>59</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="27">
+        <v>1</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="27">
+        <v>0</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="27">
+        <v>16</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="27">
+        <v>0</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="27">
+        <v>5</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="27">
+        <v>0</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="27">
+        <v>23</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="27">
+        <v>0</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="16">
+        <v>51</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="16">
+        <v>96</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="16">
+        <v>5</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A29"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -977,13 +1731,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="A1" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1011,7 +1765,7 @@
     </row>
     <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="7">
         <v>100.15639959287699</v>
@@ -1045,7 +1799,7 @@
     </row>
     <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="7">
         <v>24.530835758638101</v>
@@ -1113,7 +1867,7 @@
     </row>
     <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="8">
         <v>7.2833495241953206E-2</v>
@@ -1130,7 +1884,7 @@
     </row>
     <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1234,12 +1988,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1257,48 +2011,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="A1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="E2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>36</v>
-      </c>
       <c r="H2" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="12">
         <v>3.8259046021258598</v>
@@ -1327,7 +2081,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="12">
         <v>11.6629156353062</v>
@@ -1356,7 +2110,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="12">
         <v>3.8256224295928498</v>
@@ -1385,7 +2139,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="12">
         <v>2.3372047737642601</v>
@@ -1414,7 +2168,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="12">
         <v>1.4140390948910799</v>
@@ -1443,7 +2197,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="12">
         <v>7.7116585255798703E-2</v>
@@ -1472,7 +2226,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="12">
         <v>0.98357968718654198</v>
@@ -1501,7 +2255,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="12">
         <v>13.981264010342599</v>
@@ -1530,7 +2284,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="12">
         <v>11.4524142302475</v>
@@ -1559,7 +2313,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="12">
         <v>4.0312116339573798</v>
@@ -1588,7 +2342,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="12">
         <v>5.86416232548794</v>
@@ -1617,7 +2371,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="12">
         <v>1.8958099806787401</v>
@@ -1646,7 +2400,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="12">
         <v>-0.17397088949846501</v>
@@ -1675,7 +2429,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="12">
         <v>4.6066897736289603</v>
@@ -1704,7 +2458,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="12">
         <v>7.5536840274200898</v>
@@ -1733,7 +2487,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="12">
         <v>2.2801732314539298</v>
@@ -1762,7 +2516,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="12">
         <v>-0.29360900539779899</v>
@@ -1791,7 +2545,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="14">
         <v>0.279275362119003</v>
@@ -1819,35 +2573,35 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="25">
+      <c r="B21" s="21">
         <f>AVERAGE(B5:B20)</f>
         <v>3.7571667031956508</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="21">
         <f t="shared" ref="C21:I21" si="0">AVERAGE(C5:C20)</f>
         <v>0.7120620024421358</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="21">
         <f t="shared" si="0"/>
         <v>8.5548409148033357</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="21">
         <f t="shared" si="0"/>
         <v>0.46111424476758095</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="21">
         <f t="shared" si="0"/>
         <v>4.76863408325449</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="21">
         <f t="shared" si="0"/>
         <v>3.5772406087904352</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="21">
         <f t="shared" si="0"/>
         <v>9.9087974291531182</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="21">
         <f t="shared" si="0"/>
         <v>31.739855986406727</v>
       </c>
@@ -1994,12 +2748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2009,135 +2763,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
+      <c r="A1" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="24"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="20" t="s">
-        <v>52</v>
-      </c>
       <c r="P3" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" s="12">
         <v>20.079052846840298</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="N4" s="12">
         <v>19.382297485855101</v>
@@ -2151,22 +2905,22 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H5" s="12">
         <v>27.139027898624001</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N5" s="12">
         <v>16.541104801067799</v>
@@ -2180,25 +2934,25 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H6" s="12">
         <v>30.441160946743601</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N6" s="12">
         <v>26.502150372800301</v>
@@ -2213,22 +2967,22 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H7" s="12">
         <v>18.116015828497599</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N7" s="12">
         <v>25.834055056104699</v>
@@ -2243,25 +2997,25 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H8" s="12">
         <v>21.165528894888901</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N8" s="12">
         <v>18.666739746079202</v>
@@ -2276,16 +3030,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" s="12">
         <v>1.5558533844685001</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N9" s="12">
         <v>5.8179929364745702</v>
@@ -2300,16 +3054,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H10" s="12">
         <v>1.3339664643078</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N10" s="12">
         <v>7.2241581355289499</v>
@@ -2324,25 +3078,25 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H11" s="12">
         <v>24.024819490112701</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N11" s="12">
         <v>12.0909139155526</v>
@@ -2357,28 +3111,28 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H12" s="12">
         <v>27.687600970005601</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N12" s="12">
         <v>10.223110138722401</v>
@@ -2393,19 +3147,19 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" s="12">
         <v>10.779872100928801</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N13" s="12">
         <v>9.6749756723765099</v>
@@ -2420,22 +3174,22 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H14" s="12">
         <v>54.344361142806797</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N14" s="12">
         <v>29.8773817359647</v>
@@ -2450,19 +3204,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="12">
         <v>10.597977336528601</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N15" s="12">
         <v>7.2236421328398199</v>
@@ -2477,19 +3231,19 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="12">
         <v>23.469860468929198</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N16" s="12">
         <v>36.401189358596802</v>
@@ -2504,16 +3258,16 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" s="12">
         <v>7.5557961539220697</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N17" s="12">
         <v>3.84694004446381</v>
@@ -2528,22 +3282,22 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H18" s="12">
         <v>28.3923382760034</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N18" s="12">
         <v>17.2954425049831</v>
@@ -2558,22 +3312,22 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H19" s="12">
         <v>14.1358158157293</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N19" s="12">
         <v>15.366018274553101</v>
@@ -2588,19 +3342,19 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H20" s="12">
         <v>5.8352171120526304</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N20" s="12">
         <v>11.6712255204115</v>
@@ -2615,13 +3369,13 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -2629,13 +3383,13 @@
         <v>3.83291938858298</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N21" s="14">
         <v>13.619076800758901</v>

</xml_diff>

<commit_message>
revisions almost done, bw and color figs added
</commit_message>
<xml_diff>
--- a/tabs/alltabs.xlsx
+++ b/tabs/alltabs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="124">
   <si>
     <t>Secchi depth (m)</t>
   </si>
@@ -720,6 +720,15 @@
   <si>
     <t>ns-</t>
   </si>
+  <si>
+    <t>ave</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
 </sst>
 </file>
 
@@ -820,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -839,28 +848,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -876,12 +865,6 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -890,6 +873,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1174,7 +1178,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1192,524 +1196,525 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="19" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="22">
         <v>29</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="22">
         <v>0</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="22">
         <v>100</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="22">
         <v>1</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="22">
         <v>50</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="22">
         <v>0</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="22">
         <v>26</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="22">
         <v>8</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="22">
         <v>2</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="22">
         <v>0</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="22">
         <v>27</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="22">
         <v>0</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="22">
         <v>3</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="22">
         <v>1</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="22">
         <v>17</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="22">
         <v>0</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="22">
         <v>22</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="22">
         <v>1</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="22">
         <v>41</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="22">
         <v>3</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="22" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="22">
         <v>19</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="22">
         <v>0</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="22">
         <v>72</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="22">
         <v>0</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="22">
         <v>36</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="22">
         <v>0</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="22">
         <v>54</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="22">
         <v>1</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="22">
         <v>24</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="22">
         <v>0</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="22">
         <v>61</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="22">
         <v>1</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="22">
         <v>66</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="22">
         <v>2</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="22">
         <v>50</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="22">
         <v>11</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="22" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="22">
         <v>37</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="22">
         <v>0</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="22">
         <v>80</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="22">
         <v>1</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="22">
         <v>16</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="22">
         <v>0</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="22">
         <v>48</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="22">
         <v>0</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="22">
         <v>40</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="22">
         <v>2</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="22">
         <v>82</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="22">
         <v>4</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="22" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="22">
         <v>15</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="22">
         <v>0</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="22">
         <v>59</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="22">
         <v>0</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="22">
         <v>1</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="22">
         <v>0</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="22">
         <v>16</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="22">
         <v>0</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="22">
         <v>5</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="22">
         <v>0</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="22">
         <v>23</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="22">
         <v>0</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="19">
         <v>51</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="19">
         <v>1</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="19">
         <v>96</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="19">
         <v>5</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="19" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1731,7 +1736,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1742,13 +1747,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1769,10 +1774,10 @@
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
@@ -2043,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2062,42 +2067,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2105,28 +2110,28 @@
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="12">
         <v>3.3778251829789201</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="12">
         <v>0.571451103401588</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="12">
         <v>5.8521725074533197</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="12">
         <v>0.19693796255118001</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="12">
         <v>5.8542033567551899</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="12">
         <v>3.4726456715185399</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="12">
         <v>12.352096613156601</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="12">
         <v>31.677332397815398</v>
       </c>
     </row>
@@ -2134,548 +2139,605 @@
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="12">
         <v>11.825240859986399</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="12">
         <v>-0.46962107983352702</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="12">
         <v>12.5779082629005</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="12">
         <v>0.79718786564458899</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="12">
         <v>5.3026817947930596</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="12">
         <v>5.5554443988575599</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="12">
         <v>10.9108562204637</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="12">
         <v>46.499698322812201</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="12">
         <v>4.2520799910078404</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="12">
         <v>0.584689749626643</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="12">
         <v>2.4577654759282601</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="12">
         <v>3.4249170334015901</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="12">
         <v>1.4486927046398499</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="12">
         <v>3.3300694147374199</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="12">
         <v>21.043850885132201</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="12">
         <v>36.542065254473798</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="12">
         <v>2.02562665523917</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="12">
         <v>-5.4885511331193002E-2</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="12">
         <v>19.9385732238601</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="12">
         <v>0.50922248184473995</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="12">
         <v>9.1429901798543796</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="12">
         <v>1.2056846711076901</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="12">
         <v>16.236727905736799</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="12">
         <v>49.003939606311697</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="12">
         <v>1.43085188442867</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="12">
         <v>2.3301763278111398</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="12">
         <v>3.11275342839228</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="12">
         <v>1.02185254741496</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="12">
         <v>1.6407785738599601</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="12">
         <v>5.0388921660522099</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="12">
         <v>13.673932296993099</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="12">
         <v>28.249237224952299</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="12">
         <v>2.3986042341741101</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="12">
         <v>1.72898441141994</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="12">
         <v>8.6385217196864303</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="12">
         <v>-0.41698395845182201</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="12">
         <v>3.87611029404616</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="12">
         <v>-0.110577210207408</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="12">
         <v>0.62988218946028496</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="12">
         <v>16.7445416801277</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="12">
         <v>1.7607290957972299</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="12">
         <v>-0.164963564412279</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="12">
         <v>10.3151852463987</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="12">
         <v>9.3299791819467806E-2</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="12">
         <v>5.8749171427590401</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="12">
         <v>-1.94096718867162</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="12">
         <v>1.42090476536272</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="12">
         <v>17.3591052890532</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="12">
         <v>8.1976709662201994</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="12">
         <v>1.62568339610655</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="12">
         <v>7.7141478066885796</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="12">
         <v>1.0992104833549701</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="12">
         <v>0.68347240732845604</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="12">
         <v>2.04816249130231</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="12">
         <v>8.6825476287626007</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="12">
         <v>30.0508951797637</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="12">
         <v>10.9464226607607</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="12">
         <v>0.776829636030407</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="12">
         <v>9.6558196306275992</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="12">
         <v>-0.93719399322308405</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="12">
         <v>2.4860484088992001</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="12">
         <v>12.842547659705801</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="12">
         <v>7.8974260870158899</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="12">
         <v>43.667900089816499</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="12">
         <v>3.6912040146713698</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="12">
         <v>-0.33800829738676003</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="12">
         <v>7.6001537944145401</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="12">
         <v>-1.59994326843882E-2</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="12">
         <v>4.6458500068243396</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="12">
         <v>1.7215341233185</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="12">
         <v>5.3831333956233198</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="12">
         <v>22.687867604780902</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="12">
         <v>5.7008846417220704</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="12">
         <v>-0.17364523920998501</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="12">
         <v>11.5186972871888</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="12">
         <v>0.36185070940216701</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="12">
         <v>0.68433811314297899</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="12">
         <v>19.276787639053001</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="12">
         <v>29.004838152629599</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="12">
         <v>66.3737513039286</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="12">
         <v>2.3136193470353601</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="12">
         <v>-0.30198458109597098</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="12">
         <v>17.475789815655101</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="12">
         <v>6.8470965523870202E-3</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="12">
         <v>4.6428987354789601</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="12">
         <v>5.4016300110364197</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="12">
         <v>2.8758808819044401</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="12">
         <v>32.4146813065666</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="12">
         <v>1.6767337615153401E-2</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="12">
         <v>0.86238560487041904</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="12">
         <v>8.2031640882310999</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="12">
         <v>8.4176857442730402E-2</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="12">
         <v>15.6603020244977</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="12">
         <v>3.57459140208534</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="12">
         <v>19.794324871785999</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="12">
         <v>48.195712186528397</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="12">
         <v>4.7246352741387403</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="12">
         <v>0.41731286066055701</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="12">
         <v>5.5438929898203897</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="12">
         <v>0.58482707481429796</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="12">
         <v>1.14988698999914</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="12">
         <v>0.551420685979231</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="12">
         <v>1.6949131189897899</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="12">
         <v>14.6668889944022</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="12">
         <v>7.1402920717632297</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="12">
         <v>0.250490092786471</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="12">
         <v>9.3431121970028403</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="12">
         <v>-0.55545854861635002</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="12">
         <v>0.29091373933353099</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="12">
         <v>5.0978212662695697</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="12">
         <v>17.309497221479401</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="12">
         <v>38.8766680400187</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="12">
         <v>2.3073096591806102</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="12">
         <v>-2.7172152351906401E-2</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="12">
         <v>6.1943195319822104</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="12">
         <v>0.21681010527582201</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="12">
         <v>6.4883489890575499</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="12">
         <v>2.9236647187011902</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="12">
         <v>8.6880313325716401</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="12">
         <v>26.791312184417102</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="12">
         <v>-0.25752082120286102</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="12">
         <v>1.1094265842442199</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="12">
         <v>4.5790730284589003</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="12">
         <v>0.25690445371296899</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="12">
         <v>4.8030362830040101</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="12">
         <v>0.33397528009224697</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="12">
         <v>5.50185819945027</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="12">
         <v>16.326753007759802</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="18">
         <v>0.23580949887743699</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="18">
         <v>0.284328675356604</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="18">
         <v>5.65999075144709</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="18">
         <v>0.415673358526847</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="18">
         <v>10.117156453025</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="18">
         <v>0.37951821732826702</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="18">
         <v>2.8019183138504302</v>
       </c>
-      <c r="I20" s="26">
+      <c r="I20" s="18">
         <v>19.8943952684116</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="14">
+      <c r="A21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="11">
         <f>AVERAGE(B5:B20)</f>
         <v>3.5553116569643146</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="11">
         <f t="shared" ref="C21:I21" si="0">AVERAGE(C5:C20)</f>
         <v>0.55685299957030354</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="11">
         <f t="shared" si="0"/>
         <v>8.6219350009864328</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="11">
         <f>AVERAGE(E5:E20)</f>
         <v>0.38437225378670642</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <f t="shared" si="0"/>
         <v>4.6022338153593907</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="11">
         <f t="shared" si="0"/>
         <v>3.8546722092431351</v>
       </c>
-      <c r="H21" s="14">
-        <f t="shared" si="0"/>
+      <c r="H21" s="11">
+        <f>AVERAGE(H5:H20)</f>
         <v>10.164979202921781</v>
       </c>
-      <c r="I21" s="14">
-        <f t="shared" si="0"/>
+      <c r="I21" s="11">
+        <f>AVERAGE(I5:I20)</f>
         <v>31.740357138832053</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="11">
+        <f>MIN(B5:B20)</f>
+        <v>-0.25752082120286102</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" ref="C22:H22" si="1">MIN(C5:C20)</f>
+        <v>-0.33800829738676003</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="1"/>
+        <v>2.4577654759282601</v>
+      </c>
+      <c r="E22" s="11">
+        <f t="shared" si="1"/>
+        <v>-0.93719399322308405</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="1"/>
+        <v>0.29091373933353099</v>
+      </c>
+      <c r="G22" s="11">
+        <f t="shared" si="1"/>
+        <v>-1.94096718867162</v>
+      </c>
+      <c r="H22" s="11">
+        <f t="shared" si="1"/>
+        <v>0.62988218946028496</v>
+      </c>
+      <c r="I22" s="11">
+        <f>MIN(I5:I20)</f>
+        <v>14.6668889944022</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="11">
+        <f>MAX(B5:B20)</f>
+        <v>10.9464226607607</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" ref="C23:I23" si="2">MAX(C5:C20)</f>
+        <v>2.3301763278111398</v>
+      </c>
+      <c r="D23" s="11">
+        <f t="shared" si="2"/>
+        <v>19.9385732238601</v>
+      </c>
+      <c r="E23" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4249170334015901</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="2"/>
+        <v>15.6603020244977</v>
+      </c>
+      <c r="G23" s="11">
+        <f t="shared" si="2"/>
+        <v>19.276787639053001</v>
+      </c>
+      <c r="H23" s="11">
+        <f t="shared" si="2"/>
+        <v>29.004838152629599</v>
+      </c>
+      <c r="I23" s="11">
+        <f t="shared" si="2"/>
+        <v>66.3737513039286</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
@@ -2804,7 +2866,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2814,94 +2876,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="27" t="s">
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="27"/>
+      <c r="P2" s="28"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="I3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="29" t="s">
+      <c r="M3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="20" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2923,7 +2985,7 @@
       <c r="G4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="12">
         <v>19.610934971354101</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -2941,13 +3003,13 @@
       <c r="M4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="20">
+      <c r="N4" s="12">
         <v>19.382297485855101</v>
       </c>
-      <c r="O4" s="31">
+      <c r="O4" s="21">
         <v>21</v>
       </c>
-      <c r="P4" s="20">
+      <c r="P4" s="12">
         <v>28.177008405103098</v>
       </c>
     </row>
@@ -2967,7 +3029,7 @@
       <c r="G5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="12">
         <v>29.088729344952299</v>
       </c>
       <c r="I5" s="5"/>
@@ -2979,18 +3041,18 @@
       <c r="M5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="12">
         <v>16.541104801067799</v>
       </c>
-      <c r="O5" s="31">
+      <c r="O5" s="21">
         <v>10</v>
       </c>
-      <c r="P5" s="20">
+      <c r="P5" s="12">
         <v>34.346890677014798</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -3005,7 +3067,7 @@
       <c r="G6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="12">
         <v>32.050917324279098</v>
       </c>
       <c r="I6" s="5"/>
@@ -3019,19 +3081,19 @@
         <v>62</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="20">
+      <c r="N6" s="12">
         <v>26.502150372800301</v>
       </c>
-      <c r="O6" s="31">
+      <c r="O6" s="21">
         <v>8</v>
       </c>
-      <c r="P6" s="20">
+      <c r="P6" s="12">
         <v>28.2803784804378</v>
       </c>
-      <c r="Q6" s="12"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -3044,7 +3106,7 @@
         <v>55</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="20">
+      <c r="H7" s="12">
         <v>19.977261713928399</v>
       </c>
       <c r="I7" s="5"/>
@@ -3054,19 +3116,19 @@
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="20">
+      <c r="N7" s="12">
         <v>25.834055056104699</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="21">
         <v>12</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="12">
         <v>44.943269684689497</v>
       </c>
-      <c r="Q7" s="12"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -3079,7 +3141,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="20">
+      <c r="H8" s="12">
         <v>21.165528894888901</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -3093,19 +3155,19 @@
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="20">
+      <c r="N8" s="12">
         <v>18.666739746079202</v>
       </c>
-      <c r="O8" s="31">
+      <c r="O8" s="21">
         <v>7</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="12">
         <v>23.466356465297601</v>
       </c>
-      <c r="Q8" s="12"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="5"/>
@@ -3116,7 +3178,7 @@
         <v>56</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="20">
+      <c r="H9" s="12">
         <v>2.5009252549751602</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -3126,19 +3188,19 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="20">
+      <c r="N9" s="12">
         <v>5.8179929364745702</v>
       </c>
-      <c r="O9" s="31">
+      <c r="O9" s="21">
         <v>4</v>
       </c>
-      <c r="P9" s="20">
+      <c r="P9" s="12">
         <v>13.033936992985501</v>
       </c>
-      <c r="Q9" s="12"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -3149,7 +3211,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="20">
+      <c r="H10" s="12">
         <v>1.3339664643078</v>
       </c>
       <c r="I10" s="5"/>
@@ -3159,19 +3221,19 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="20">
+      <c r="N10" s="12">
         <v>7.2241581355289499</v>
       </c>
-      <c r="O10" s="31">
+      <c r="O10" s="21">
         <v>7</v>
       </c>
-      <c r="P10" s="20">
+      <c r="P10" s="12">
         <v>15.670039965848799</v>
       </c>
-      <c r="Q10" s="12"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -3188,7 +3250,7 @@
       <c r="G11" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="12">
         <v>20.027591569640101</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -3200,19 +3262,19 @@
         <v>55</v>
       </c>
       <c r="M11" s="5"/>
-      <c r="N11" s="20">
+      <c r="N11" s="12">
         <v>12.0909139155526</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="21">
         <v>5</v>
       </c>
-      <c r="P11" s="20">
+      <c r="P11" s="12">
         <v>19.128330334081902</v>
       </c>
-      <c r="Q11" s="12"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3229,7 +3291,7 @@
       <c r="G12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="12">
         <v>30.749202414259301</v>
       </c>
       <c r="I12" s="5" t="s">
@@ -3241,19 +3303,19 @@
         <v>62</v>
       </c>
       <c r="M12" s="5"/>
-      <c r="N12" s="20">
+      <c r="N12" s="12">
         <v>10.223110138722401</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="21">
         <v>8</v>
       </c>
-      <c r="P12" s="20">
+      <c r="P12" s="12">
         <v>32.881841786248501</v>
       </c>
-      <c r="Q12" s="12"/>
+      <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="5"/>
@@ -3266,7 +3328,7 @@
       <c r="G13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="12">
         <v>10.779872100928801</v>
       </c>
       <c r="I13" s="5"/>
@@ -3276,19 +3338,19 @@
       <c r="M13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N13" s="20">
+      <c r="N13" s="12">
         <v>9.6749756723765099</v>
       </c>
-      <c r="O13" s="31">
+      <c r="O13" s="21">
         <v>8</v>
       </c>
-      <c r="P13" s="20">
+      <c r="P13" s="12">
         <v>20.515239592268099</v>
       </c>
-      <c r="Q13" s="12"/>
+      <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -3303,7 +3365,7 @@
       <c r="G14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="12">
         <v>54.344361142806797</v>
       </c>
       <c r="I14" s="5"/>
@@ -3313,19 +3375,19 @@
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="20">
+      <c r="N14" s="12">
         <v>29.8773817359647</v>
       </c>
-      <c r="O14" s="31">
+      <c r="O14" s="21">
         <v>19</v>
       </c>
-      <c r="P14" s="20">
+      <c r="P14" s="12">
         <v>60.484661192014201</v>
       </c>
-      <c r="Q14" s="12"/>
+      <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="5"/>
@@ -3338,7 +3400,7 @@
       <c r="G15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="12">
         <v>10.597977336528601</v>
       </c>
       <c r="I15" s="5"/>
@@ -3348,19 +3410,19 @@
       <c r="M15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="12">
         <v>7.2236421328398199</v>
       </c>
-      <c r="O15" s="31">
+      <c r="O15" s="21">
         <v>9</v>
       </c>
-      <c r="P15" s="20">
+      <c r="P15" s="12">
         <v>29.2930863053368</v>
       </c>
-      <c r="Q15" s="12"/>
+      <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3371,7 +3433,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="20">
+      <c r="H16" s="12">
         <v>23.469860468929198</v>
       </c>
       <c r="I16" s="5" t="s">
@@ -3383,19 +3445,19 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="20">
+      <c r="N16" s="12">
         <v>36.401189358596802</v>
       </c>
-      <c r="O16" s="31">
+      <c r="O16" s="21">
         <v>8</v>
       </c>
-      <c r="P16" s="20">
+      <c r="P16" s="12">
         <v>47.982729781038202</v>
       </c>
-      <c r="Q16" s="12"/>
+      <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="5"/>
@@ -3406,7 +3468,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="20">
+      <c r="H17" s="12">
         <v>7.5557961539220697</v>
       </c>
       <c r="I17" s="5"/>
@@ -3416,19 +3478,19 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="20">
+      <c r="N17" s="12">
         <v>3.84694004446381</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O17" s="21">
         <v>3</v>
       </c>
-      <c r="P17" s="20">
+      <c r="P17" s="12">
         <v>8.9401137847885508</v>
       </c>
-      <c r="Q17" s="12"/>
+      <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -3441,7 +3503,7 @@
         <v>61</v>
       </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="20">
+      <c r="H18" s="12">
         <v>28.9921520108959</v>
       </c>
       <c r="I18" s="5"/>
@@ -3451,19 +3513,19 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="20">
+      <c r="N18" s="12">
         <v>17.2954425049831</v>
       </c>
-      <c r="O18" s="31">
+      <c r="O18" s="21">
         <v>9</v>
       </c>
-      <c r="P18" s="20">
+      <c r="P18" s="12">
         <v>32.041344424085402</v>
       </c>
-      <c r="Q18" s="12"/>
+      <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="16" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -3476,7 +3538,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="20">
+      <c r="H19" s="12">
         <v>14.1358158157293</v>
       </c>
       <c r="I19" s="5" t="s">
@@ -3488,19 +3550,19 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="20">
+      <c r="N19" s="12">
         <v>15.366018274553101</v>
       </c>
-      <c r="O19" s="31">
+      <c r="O19" s="21">
         <v>6</v>
       </c>
-      <c r="P19" s="20">
+      <c r="P19" s="12">
         <v>24.294364572312599</v>
       </c>
-      <c r="Q19" s="12"/>
+      <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="16" t="s">
         <v>60</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3511,7 +3573,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="20">
+      <c r="H20" s="12">
         <v>5.8352171120526304</v>
       </c>
       <c r="I20" s="5" t="s">
@@ -3523,19 +3585,19 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="20">
+      <c r="N20" s="12">
         <v>11.6712255204115</v>
       </c>
-      <c r="O20" s="31">
+      <c r="O20" s="21">
         <v>3</v>
       </c>
-      <c r="P20" s="20">
+      <c r="P20" s="12">
         <v>13.664110831088401</v>
       </c>
-      <c r="Q20" s="12"/>
+      <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="2"/>
@@ -3546,7 +3608,7 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="26">
+      <c r="H21" s="18">
         <v>3.83291938858298</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -3558,13 +3620,13 @@
       <c r="M21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="N21" s="26">
+      <c r="N21" s="18">
         <v>13.619076800758901</v>
       </c>
-      <c r="O21" s="30">
+      <c r="O21" s="20">
         <v>5</v>
       </c>
-      <c r="P21" s="26">
+      <c r="P21" s="18">
         <v>18.958583735650802</v>
       </c>
     </row>

</xml_diff>